<commit_message>
From Work test SQL send
</commit_message>
<xml_diff>
--- a/app/Imports/data-excel-2025.xlsx
+++ b/app/Imports/data-excel-2025.xlsx
@@ -1765,7 +1765,7 @@
   <dimension ref="A1:AM28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1"/>
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,7 +2056,7 @@
         <v>2</v>
       </c>
       <c r="L3" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M3" s="2">
         <v>3</v>
@@ -2159,7 +2159,7 @@
         <v>3</v>
       </c>
       <c r="L4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2">
@@ -2256,7 +2256,7 @@
         <v>4</v>
       </c>
       <c r="L5" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M5" s="2">
         <v>7</v>
@@ -2359,7 +2359,7 @@
         <v>4</v>
       </c>
       <c r="L6" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M6" s="2">
         <v>9</v>
@@ -2462,7 +2462,7 @@
         <v>4</v>
       </c>
       <c r="L7" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M7" s="2">
         <v>11</v>
@@ -2565,7 +2565,7 @@
         <v>4</v>
       </c>
       <c r="L8" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M8" s="2">
         <v>13</v>
@@ -2668,7 +2668,7 @@
         <v>2</v>
       </c>
       <c r="L9" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M9" s="2">
         <v>15</v>
@@ -2771,7 +2771,7 @@
         <v>2</v>
       </c>
       <c r="L10" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M10" s="2">
         <v>17</v>
@@ -2874,7 +2874,7 @@
         <v>2</v>
       </c>
       <c r="L11" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M11" s="2">
         <v>19</v>
@@ -2977,7 +2977,7 @@
         <v>2</v>
       </c>
       <c r="L12" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M12" s="2">
         <v>21</v>
@@ -3080,7 +3080,7 @@
         <v>2</v>
       </c>
       <c r="L13" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M13" s="2">
         <v>23</v>
@@ -3183,7 +3183,7 @@
         <v>2</v>
       </c>
       <c r="L14" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M14" s="2">
         <v>25</v>
@@ -3286,7 +3286,7 @@
         <v>2</v>
       </c>
       <c r="L15" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M15" s="2">
         <v>27</v>
@@ -4388,7 +4388,7 @@
         <v>3</v>
       </c>
       <c r="L25" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2">
@@ -4485,7 +4485,7 @@
         <v>3</v>
       </c>
       <c r="L26" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2">
@@ -4582,7 +4582,7 @@
         <v>3</v>
       </c>
       <c r="L27" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2">
@@ -4679,7 +4679,7 @@
         <v>3</v>
       </c>
       <c r="L28" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2">

</xml_diff>

<commit_message>
From cafe 23/01/2025 at 21H00
</commit_message>
<xml_diff>
--- a/app/Imports/data-excel-2025.xlsx
+++ b/app/Imports/data-excel-2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\projects\grace-app\back_grace\app\Imports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Grace Project\grace_back\app\Imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1765,7 +1765,7 @@
   <dimension ref="A1:AM28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
from work 05/02/2025 at 16h00
</commit_message>
<xml_diff>
--- a/app/Imports/data-excel-2025.xlsx
+++ b/app/Imports/data-excel-2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Grace Project\grace_back\app\Imports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\projects\grace-app\back_grace\app\Imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$AM$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$1:$AO$28</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="461">
   <si>
     <t>nom</t>
   </si>
@@ -1404,6 +1404,12 @@
   </si>
   <si>
     <t>date_jujement</t>
+  </si>
+  <si>
+    <t>objetdemande_id</t>
+  </si>
+  <si>
+    <t>user_id</t>
   </si>
 </sst>
 </file>
@@ -1762,187 +1768,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM28"/>
+  <dimension ref="A1:AO28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="15.7109375" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="21" width="14.140625" customWidth="1"/>
-    <col min="22" max="22" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="27" width="13.5703125" style="5" customWidth="1"/>
-    <col min="28" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="10.85546875" customWidth="1"/>
-    <col min="31" max="31" width="8" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.42578125" customWidth="1"/>
-    <col min="35" max="35" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="14.140625" customWidth="1"/>
+    <col min="24" max="24" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="29" width="13.5703125" style="5" customWidth="1"/>
+    <col min="30" max="30" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="10.85546875" customWidth="1"/>
+    <col min="33" max="33" width="8" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.42578125" customWidth="1"/>
+    <col min="37" max="37" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
       <c r="I2" s="2">
         <v>1</v>
       </c>
@@ -1958,94 +1968,98 @@
       <c r="M2" s="2">
         <v>1</v>
       </c>
-      <c r="N2" s="2">
-        <v>1</v>
-      </c>
+      <c r="N2" s="2"/>
       <c r="O2" s="2">
         <v>1</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>1</v>
+      </c>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="2" t="s">
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="AG2" s="2">
         <v>123</v>
       </c>
-      <c r="AF2" s="2">
+      <c r="AH2" s="2">
         <v>2908</v>
       </c>
-      <c r="AG2" s="2">
+      <c r="AI2" s="2">
         <v>2003</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="AK2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="2">
-        <v>1</v>
-      </c>
       <c r="AM2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO2" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
       <c r="I3" s="2">
         <v>1</v>
       </c>
@@ -2053,102 +2067,106 @@
         <v>1</v>
       </c>
       <c r="K3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M3" s="2">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2">
         <v>3</v>
       </c>
-      <c r="N3" s="2">
-        <v>2</v>
-      </c>
-      <c r="O3" s="2">
-        <v>1</v>
-      </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
+      <c r="P3" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>1</v>
+      </c>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="4" t="s">
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="Y3" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="Z3" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="AA3" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="2" t="s">
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AF3" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="AE3" s="2">
+      <c r="AG3" s="2">
         <v>123</v>
       </c>
-      <c r="AF3" s="2">
+      <c r="AH3" s="2">
         <v>2908</v>
       </c>
-      <c r="AG3" s="2">
+      <c r="AI3" s="2">
         <v>2003</v>
       </c>
-      <c r="AH3" s="4" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="AI3" s="4" t="s">
+      <c r="AK3" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AL3" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="AK3" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL3" s="2">
-        <v>1</v>
-      </c>
       <c r="AM3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
       <c r="I4" s="2">
         <v>1</v>
       </c>
@@ -2156,96 +2174,102 @@
         <v>1</v>
       </c>
       <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
         <v>3</v>
       </c>
-      <c r="L4" s="2">
-        <v>2</v>
-      </c>
-      <c r="M4" s="2"/>
+      <c r="M4" s="2">
+        <v>2</v>
+      </c>
       <c r="N4" s="2">
-        <v>2</v>
-      </c>
-      <c r="O4" s="2">
-        <v>1</v>
-      </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>1</v>
+      </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
-      <c r="V4" s="4" t="s">
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="Y4" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
-      <c r="AB4" s="2" t="s">
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AC4" s="2" t="s">
+      <c r="AE4" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="AD4" s="2" t="s">
+      <c r="AF4" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="AE4" s="2">
+      <c r="AG4" s="2">
         <v>123</v>
       </c>
-      <c r="AF4" s="2">
+      <c r="AH4" s="2">
         <v>2908</v>
       </c>
-      <c r="AG4" s="2">
+      <c r="AI4" s="2">
         <v>2003</v>
       </c>
-      <c r="AH4" s="4" t="s">
+      <c r="AJ4" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="AI4" s="4" t="s">
+      <c r="AK4" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="AJ4" s="2" t="s">
+      <c r="AL4" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="AK4" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL4" s="2">
-        <v>1</v>
-      </c>
       <c r="AM4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO4" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
       <c r="I5" s="2">
         <v>1</v>
       </c>
@@ -2253,102 +2277,106 @@
         <v>1</v>
       </c>
       <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
         <v>4</v>
       </c>
-      <c r="L5" s="2">
-        <v>1</v>
-      </c>
       <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2">
         <v>7</v>
       </c>
-      <c r="N5" s="2">
-        <v>2</v>
-      </c>
-      <c r="O5" s="2">
-        <v>1</v>
-      </c>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
+      <c r="P5" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>1</v>
+      </c>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
-      <c r="V5" s="4" t="s">
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="W5" s="4" t="s">
+      <c r="Y5" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="X5" s="4" t="s">
+      <c r="Z5" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y5" s="4" t="s">
+      <c r="AA5" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="2" t="s">
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AC5" s="2" t="s">
+      <c r="AE5" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="AD5" s="2" t="s">
+      <c r="AF5" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="AE5" s="2">
+      <c r="AG5" s="2">
         <v>123</v>
       </c>
-      <c r="AF5" s="2">
+      <c r="AH5" s="2">
         <v>2908</v>
       </c>
-      <c r="AG5" s="2">
+      <c r="AI5" s="2">
         <v>2003</v>
       </c>
-      <c r="AH5" s="4" t="s">
+      <c r="AJ5" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="AI5" s="4" t="s">
+      <c r="AK5" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="AJ5" s="2" t="s">
+      <c r="AL5" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="AK5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL5" s="2">
-        <v>1</v>
-      </c>
       <c r="AM5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO5" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
       <c r="I6" s="2">
         <v>1</v>
       </c>
@@ -2356,102 +2384,106 @@
         <v>1</v>
       </c>
       <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
         <v>4</v>
       </c>
-      <c r="L6" s="2">
-        <v>1</v>
-      </c>
       <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2">
         <v>9</v>
       </c>
-      <c r="N6" s="2">
-        <v>2</v>
-      </c>
-      <c r="O6" s="2">
-        <v>1</v>
-      </c>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
+      <c r="P6" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>1</v>
+      </c>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
-      <c r="V6" s="4" t="s">
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="W6" s="4" t="s">
+      <c r="Y6" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="X6" s="4" t="s">
+      <c r="Z6" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y6" s="4" t="s">
+      <c r="AA6" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="2" t="s">
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AC6" s="2" t="s">
+      <c r="AE6" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="AD6" s="2" t="s">
+      <c r="AF6" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="AE6" s="2">
+      <c r="AG6" s="2">
         <v>123</v>
       </c>
-      <c r="AF6" s="2">
+      <c r="AH6" s="2">
         <v>2908</v>
       </c>
-      <c r="AG6" s="2">
+      <c r="AI6" s="2">
         <v>2003</v>
       </c>
-      <c r="AH6" s="4" t="s">
+      <c r="AJ6" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="AI6" s="4" t="s">
+      <c r="AK6" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="AJ6" s="2" t="s">
+      <c r="AL6" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="AK6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL6" s="2">
-        <v>1</v>
-      </c>
       <c r="AM6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO6" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
       <c r="I7" s="2">
         <v>1</v>
       </c>
@@ -2459,102 +2491,106 @@
         <v>1</v>
       </c>
       <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2">
         <v>4</v>
       </c>
-      <c r="L7" s="2">
-        <v>1</v>
-      </c>
       <c r="M7" s="2">
+        <v>1</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2">
         <v>11</v>
       </c>
-      <c r="N7" s="2">
-        <v>2</v>
-      </c>
-      <c r="O7" s="2">
-        <v>1</v>
-      </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
+      <c r="P7" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>1</v>
+      </c>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
-      <c r="V7" s="4" t="s">
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="W7" s="4" t="s">
+      <c r="Y7" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="X7" s="4" t="s">
+      <c r="Z7" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y7" s="4" t="s">
+      <c r="AA7" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="Z7" s="4"/>
-      <c r="AA7" s="4"/>
-      <c r="AB7" s="2" t="s">
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AC7" s="2" t="s">
+      <c r="AE7" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="AD7" s="2" t="s">
+      <c r="AF7" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="AE7" s="2">
+      <c r="AG7" s="2">
         <v>123</v>
       </c>
-      <c r="AF7" s="2">
+      <c r="AH7" s="2">
         <v>2908</v>
       </c>
-      <c r="AG7" s="2">
+      <c r="AI7" s="2">
         <v>2003</v>
       </c>
-      <c r="AH7" s="4" t="s">
+      <c r="AJ7" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="AI7" s="4" t="s">
+      <c r="AK7" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="AJ7" s="2" t="s">
+      <c r="AL7" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="AK7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL7" s="2">
-        <v>1</v>
-      </c>
       <c r="AM7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO7" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="H8" s="2">
-        <v>1</v>
-      </c>
       <c r="I8" s="2">
         <v>1</v>
       </c>
@@ -2562,102 +2598,106 @@
         <v>1</v>
       </c>
       <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2">
         <v>4</v>
       </c>
-      <c r="L8" s="2">
-        <v>1</v>
-      </c>
       <c r="M8" s="2">
+        <v>1</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2">
         <v>13</v>
       </c>
-      <c r="N8" s="2">
-        <v>2</v>
-      </c>
-      <c r="O8" s="2">
-        <v>1</v>
-      </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
+      <c r="P8" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>1</v>
+      </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
-      <c r="V8" s="4" t="s">
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="W8" s="4" t="s">
+      <c r="Y8" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="X8" s="4" t="s">
+      <c r="Z8" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y8" s="4" t="s">
+      <c r="AA8" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="Z8" s="4"/>
-      <c r="AA8" s="4"/>
-      <c r="AB8" s="2" t="s">
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="4"/>
+      <c r="AD8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AC8" s="2" t="s">
+      <c r="AE8" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="AD8" s="2" t="s">
+      <c r="AF8" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="AE8" s="2">
+      <c r="AG8" s="2">
         <v>123</v>
       </c>
-      <c r="AF8" s="2">
+      <c r="AH8" s="2">
         <v>2908</v>
       </c>
-      <c r="AG8" s="2">
+      <c r="AI8" s="2">
         <v>2003</v>
       </c>
-      <c r="AH8" s="4" t="s">
+      <c r="AJ8" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="AI8" s="4" t="s">
+      <c r="AK8" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="AJ8" s="2" t="s">
+      <c r="AL8" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="AK8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL8" s="2">
-        <v>1</v>
-      </c>
       <c r="AM8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO8" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="H9" s="2">
-        <v>1</v>
-      </c>
       <c r="I9" s="2">
         <v>1</v>
       </c>
@@ -2665,102 +2705,106 @@
         <v>1</v>
       </c>
       <c r="K9" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M9" s="2">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2">
         <v>15</v>
       </c>
-      <c r="N9" s="2">
-        <v>2</v>
-      </c>
-      <c r="O9" s="2">
-        <v>1</v>
-      </c>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
+      <c r="P9" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>1</v>
+      </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
-      <c r="V9" s="4" t="s">
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="W9" s="4" t="s">
+      <c r="Y9" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="X9" s="4" t="s">
+      <c r="Z9" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y9" s="4" t="s">
+      <c r="AA9" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="Z9" s="4"/>
-      <c r="AA9" s="4"/>
-      <c r="AB9" s="2" t="s">
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AC9" s="2" t="s">
+      <c r="AE9" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="AD9" s="2" t="s">
+      <c r="AF9" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="AE9" s="2">
+      <c r="AG9" s="2">
         <v>123</v>
       </c>
-      <c r="AF9" s="2">
+      <c r="AH9" s="2">
         <v>2908</v>
       </c>
-      <c r="AG9" s="2">
+      <c r="AI9" s="2">
         <v>2003</v>
       </c>
-      <c r="AH9" s="4" t="s">
+      <c r="AJ9" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="AI9" s="4" t="s">
+      <c r="AK9" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="AJ9" s="2" t="s">
+      <c r="AL9" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="AK9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL9" s="2">
-        <v>1</v>
-      </c>
       <c r="AM9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO9" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H10" s="2">
-        <v>1</v>
-      </c>
       <c r="I10" s="2">
         <v>1</v>
       </c>
@@ -2768,102 +2812,106 @@
         <v>1</v>
       </c>
       <c r="K10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10" s="2">
+        <v>1</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2">
         <v>17</v>
       </c>
-      <c r="N10" s="2">
-        <v>2</v>
-      </c>
-      <c r="O10" s="2">
-        <v>1</v>
-      </c>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
+      <c r="P10" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>1</v>
+      </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
-      <c r="V10" s="4" t="s">
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="W10" s="4" t="s">
+      <c r="Y10" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="X10" s="4" t="s">
+      <c r="Z10" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y10" s="4" t="s">
+      <c r="AA10" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="Z10" s="4"/>
-      <c r="AA10" s="4"/>
-      <c r="AB10" s="2" t="s">
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="4"/>
+      <c r="AD10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AC10" s="2" t="s">
+      <c r="AE10" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="AD10" s="2" t="s">
+      <c r="AF10" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="AE10" s="2">
+      <c r="AG10" s="2">
         <v>123</v>
       </c>
-      <c r="AF10" s="2">
+      <c r="AH10" s="2">
         <v>2908</v>
       </c>
-      <c r="AG10" s="2">
+      <c r="AI10" s="2">
         <v>2003</v>
       </c>
-      <c r="AH10" s="4" t="s">
+      <c r="AJ10" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="AI10" s="4" t="s">
+      <c r="AK10" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="AJ10" s="2" t="s">
+      <c r="AL10" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="AK10" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL10" s="2">
-        <v>1</v>
-      </c>
       <c r="AM10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO10" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="H11" s="2">
-        <v>1</v>
-      </c>
       <c r="I11" s="2">
         <v>1</v>
       </c>
@@ -2871,102 +2919,106 @@
         <v>1</v>
       </c>
       <c r="K11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M11" s="2">
+        <v>1</v>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2">
         <v>19</v>
       </c>
-      <c r="N11" s="2">
-        <v>1</v>
-      </c>
-      <c r="O11" s="2">
-        <v>1</v>
-      </c>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
+      <c r="P11" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>1</v>
+      </c>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
-      <c r="V11" s="4" t="s">
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="W11" s="4" t="s">
+      <c r="Y11" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="X11" s="4" t="s">
+      <c r="Z11" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y11" s="4" t="s">
+      <c r="AA11" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="Z11" s="4"/>
-      <c r="AA11" s="4"/>
-      <c r="AB11" s="2" t="s">
+      <c r="AB11" s="4"/>
+      <c r="AC11" s="4"/>
+      <c r="AD11" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AC11" s="2" t="s">
+      <c r="AE11" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="AD11" s="2" t="s">
+      <c r="AF11" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="AE11" s="2">
+      <c r="AG11" s="2">
         <v>123</v>
       </c>
-      <c r="AF11" s="2">
+      <c r="AH11" s="2">
         <v>2908</v>
       </c>
-      <c r="AG11" s="2">
+      <c r="AI11" s="2">
         <v>2003</v>
       </c>
-      <c r="AH11" s="4" t="s">
+      <c r="AJ11" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="AI11" s="4" t="s">
+      <c r="AK11" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="AJ11" s="2" t="s">
+      <c r="AL11" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="AK11" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL11" s="2">
-        <v>1</v>
-      </c>
       <c r="AM11" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN11" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO11" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="H12" s="2">
-        <v>1</v>
-      </c>
       <c r="I12" s="2">
         <v>1</v>
       </c>
@@ -2974,102 +3026,106 @@
         <v>1</v>
       </c>
       <c r="K12" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12" s="2">
+        <v>1</v>
+      </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2">
         <v>21</v>
       </c>
-      <c r="N12" s="2">
-        <v>1</v>
-      </c>
-      <c r="O12" s="2">
-        <v>1</v>
-      </c>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
+      <c r="P12" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>1</v>
+      </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
-      <c r="V12" s="4" t="s">
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="W12" s="4" t="s">
+      <c r="Y12" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="X12" s="4" t="s">
+      <c r="Z12" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y12" s="4" t="s">
+      <c r="AA12" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
-      <c r="AB12" s="2" t="s">
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AC12" s="2" t="s">
+      <c r="AE12" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="AD12" s="2" t="s">
+      <c r="AF12" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="AE12" s="2">
+      <c r="AG12" s="2">
         <v>123</v>
       </c>
-      <c r="AF12" s="2">
+      <c r="AH12" s="2">
         <v>2908</v>
       </c>
-      <c r="AG12" s="2">
+      <c r="AI12" s="2">
         <v>2003</v>
       </c>
-      <c r="AH12" s="4" t="s">
+      <c r="AJ12" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="AI12" s="4" t="s">
+      <c r="AK12" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="AJ12" s="2" t="s">
+      <c r="AL12" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="AK12" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL12" s="2">
-        <v>1</v>
-      </c>
       <c r="AM12" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN12" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO12" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="H13" s="2">
-        <v>1</v>
-      </c>
       <c r="I13" s="2">
         <v>1</v>
       </c>
@@ -3077,102 +3133,106 @@
         <v>1</v>
       </c>
       <c r="K13" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M13" s="2">
+        <v>1</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2">
         <v>23</v>
       </c>
-      <c r="N13" s="2">
-        <v>1</v>
-      </c>
-      <c r="O13" s="2">
-        <v>1</v>
-      </c>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
+      <c r="P13" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>1</v>
+      </c>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
-      <c r="V13" s="4" t="s">
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="W13" s="4" t="s">
+      <c r="Y13" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="X13" s="4" t="s">
+      <c r="Z13" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y13" s="4" t="s">
+      <c r="AA13" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="Z13" s="4"/>
-      <c r="AA13" s="4"/>
-      <c r="AB13" s="2" t="s">
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="AC13" s="2" t="s">
+      <c r="AE13" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="AD13" s="2" t="s">
+      <c r="AF13" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="AE13" s="2">
+      <c r="AG13" s="2">
         <v>123</v>
       </c>
-      <c r="AF13" s="2">
+      <c r="AH13" s="2">
         <v>2908</v>
       </c>
-      <c r="AG13" s="2">
+      <c r="AI13" s="2">
         <v>2003</v>
       </c>
-      <c r="AH13" s="4" t="s">
+      <c r="AJ13" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="AI13" s="4" t="s">
+      <c r="AK13" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="AJ13" s="2" t="s">
+      <c r="AL13" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="AK13" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL13" s="2">
-        <v>1</v>
-      </c>
       <c r="AM13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO13" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="H14" s="2">
-        <v>1</v>
-      </c>
       <c r="I14" s="2">
         <v>1</v>
       </c>
@@ -3180,102 +3240,106 @@
         <v>1</v>
       </c>
       <c r="K14" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L14" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M14" s="2">
+        <v>1</v>
+      </c>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2">
         <v>25</v>
       </c>
-      <c r="N14" s="2">
-        <v>1</v>
-      </c>
-      <c r="O14" s="2">
-        <v>1</v>
-      </c>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
+      <c r="P14" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>1</v>
+      </c>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
-      <c r="V14" s="4" t="s">
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="W14" s="4" t="s">
+      <c r="Y14" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="X14" s="4" t="s">
+      <c r="Z14" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y14" s="4" t="s">
+      <c r="AA14" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="4"/>
-      <c r="AB14" s="2" t="s">
+      <c r="AB14" s="4"/>
+      <c r="AC14" s="4"/>
+      <c r="AD14" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="AC14" s="2" t="s">
+      <c r="AE14" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="AD14" s="2" t="s">
+      <c r="AF14" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="AE14" s="2">
+      <c r="AG14" s="2">
         <v>123</v>
       </c>
-      <c r="AF14" s="2">
+      <c r="AH14" s="2">
         <v>2908</v>
       </c>
-      <c r="AG14" s="2">
+      <c r="AI14" s="2">
         <v>2003</v>
       </c>
-      <c r="AH14" s="4" t="s">
+      <c r="AJ14" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="AI14" s="4" t="s">
+      <c r="AK14" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="AJ14" s="2" t="s">
+      <c r="AL14" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="AK14" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL14" s="2">
-        <v>1</v>
-      </c>
       <c r="AM14" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN14" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO14" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H15" s="2">
-        <v>1</v>
-      </c>
       <c r="I15" s="2">
         <v>1</v>
       </c>
@@ -3283,102 +3347,106 @@
         <v>1</v>
       </c>
       <c r="K15" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L15" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M15" s="2">
+        <v>1</v>
+      </c>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2">
         <v>27</v>
       </c>
-      <c r="N15" s="2">
-        <v>1</v>
-      </c>
-      <c r="O15" s="2">
-        <v>1</v>
-      </c>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
+      <c r="P15" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>1</v>
+      </c>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
-      <c r="V15" s="4" t="s">
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="W15" s="4" t="s">
+      <c r="Y15" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="X15" s="4" t="s">
+      <c r="Z15" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y15" s="4" t="s">
+      <c r="AA15" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
-      <c r="AB15" s="2" t="s">
+      <c r="AB15" s="4"/>
+      <c r="AC15" s="4"/>
+      <c r="AD15" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AC15" s="2" t="s">
+      <c r="AE15" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="AD15" s="2" t="s">
+      <c r="AF15" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="AE15" s="2">
+      <c r="AG15" s="2">
         <v>123</v>
       </c>
-      <c r="AF15" s="2">
+      <c r="AH15" s="2">
         <v>2908</v>
       </c>
-      <c r="AG15" s="2">
+      <c r="AI15" s="2">
         <v>2003</v>
       </c>
-      <c r="AH15" s="4" t="s">
+      <c r="AJ15" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="AI15" s="4" t="s">
+      <c r="AK15" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="AJ15" s="2" t="s">
+      <c r="AL15" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="AK15" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL15" s="2">
-        <v>1</v>
-      </c>
       <c r="AM15" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN15" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO15" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="H16" s="2">
-        <v>1</v>
-      </c>
       <c r="I16" s="2">
         <v>1</v>
       </c>
@@ -3392,108 +3460,112 @@
         <v>1</v>
       </c>
       <c r="M16" s="2">
+        <v>1</v>
+      </c>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2">
         <v>29</v>
       </c>
-      <c r="N16" s="2">
-        <v>1</v>
-      </c>
-      <c r="O16" s="2">
-        <v>2</v>
-      </c>
-      <c r="P16" s="6" t="s">
+      <c r="P16" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>2</v>
+      </c>
+      <c r="R16" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="Q16" s="6" t="s">
+      <c r="S16" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="R16" s="2" t="s">
+      <c r="T16" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="S16" s="2" t="s">
+      <c r="U16" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="T16" s="2">
+      <c r="V16" s="2">
         <v>98</v>
       </c>
-      <c r="U16" s="2">
-        <v>2</v>
-      </c>
-      <c r="V16" s="4" t="s">
+      <c r="W16" s="2">
+        <v>2</v>
+      </c>
+      <c r="X16" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="W16" s="4" t="s">
+      <c r="Y16" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="X16" s="4" t="s">
+      <c r="Z16" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y16" s="4" t="s">
+      <c r="AA16" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4"/>
-      <c r="AB16" s="2" t="s">
+      <c r="AB16" s="4"/>
+      <c r="AC16" s="4"/>
+      <c r="AD16" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AC16" s="2" t="s">
+      <c r="AE16" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="AD16" s="2" t="s">
+      <c r="AF16" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="AE16" s="2">
+      <c r="AG16" s="2">
         <v>123</v>
       </c>
-      <c r="AF16" s="2">
+      <c r="AH16" s="2">
         <v>2908</v>
       </c>
-      <c r="AG16" s="2">
+      <c r="AI16" s="2">
         <v>2003</v>
       </c>
-      <c r="AH16" s="4" t="s">
+      <c r="AJ16" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="AI16" s="4" t="s">
+      <c r="AK16" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="AJ16" s="2" t="s">
+      <c r="AL16" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="AK16" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL16" s="2">
-        <v>1</v>
-      </c>
       <c r="AM16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO16" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="H17" s="2">
-        <v>1</v>
-      </c>
       <c r="I17" s="2">
         <v>1</v>
       </c>
@@ -3507,108 +3579,112 @@
         <v>1</v>
       </c>
       <c r="M17" s="2">
+        <v>1</v>
+      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2">
         <v>31</v>
       </c>
-      <c r="N17" s="2">
-        <v>1</v>
-      </c>
-      <c r="O17" s="2">
-        <v>2</v>
-      </c>
-      <c r="P17" s="6" t="s">
+      <c r="P17" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>2</v>
+      </c>
+      <c r="R17" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="Q17" s="6" t="s">
+      <c r="S17" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="R17" s="2" t="s">
+      <c r="T17" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="S17" s="2" t="s">
+      <c r="U17" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="T17" s="2">
+      <c r="V17" s="2">
         <v>98</v>
       </c>
-      <c r="U17" s="2">
-        <v>2</v>
-      </c>
-      <c r="V17" s="4" t="s">
+      <c r="W17" s="2">
+        <v>2</v>
+      </c>
+      <c r="X17" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="W17" s="4" t="s">
+      <c r="Y17" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="X17" s="4" t="s">
+      <c r="Z17" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y17" s="4" t="s">
+      <c r="AA17" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="Z17" s="4"/>
-      <c r="AA17" s="4"/>
-      <c r="AB17" s="2" t="s">
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AC17" s="2" t="s">
+      <c r="AE17" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="AD17" s="2" t="s">
+      <c r="AF17" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="AE17" s="2">
+      <c r="AG17" s="2">
         <v>123</v>
       </c>
-      <c r="AF17" s="2">
+      <c r="AH17" s="2">
         <v>2908</v>
       </c>
-      <c r="AG17" s="2">
+      <c r="AI17" s="2">
         <v>2003</v>
       </c>
-      <c r="AH17" s="4" t="s">
+      <c r="AJ17" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="AI17" s="4" t="s">
+      <c r="AK17" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="AJ17" s="2" t="s">
+      <c r="AL17" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="AK17" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL17" s="2">
-        <v>1</v>
-      </c>
       <c r="AM17" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN17" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO17" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="G18" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="H18" s="2">
-        <v>1</v>
-      </c>
       <c r="I18" s="2">
         <v>1</v>
       </c>
@@ -3622,108 +3698,112 @@
         <v>1</v>
       </c>
       <c r="M18" s="2">
+        <v>1</v>
+      </c>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2">
         <v>33</v>
       </c>
-      <c r="N18" s="2">
-        <v>1</v>
-      </c>
-      <c r="O18" s="2">
-        <v>2</v>
-      </c>
-      <c r="P18" s="6" t="s">
+      <c r="P18" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>2</v>
+      </c>
+      <c r="R18" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="Q18" s="6" t="s">
+      <c r="S18" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="R18" s="2" t="s">
+      <c r="T18" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="S18" s="2" t="s">
+      <c r="U18" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="T18" s="2">
+      <c r="V18" s="2">
         <v>98</v>
       </c>
-      <c r="U18" s="2">
-        <v>2</v>
-      </c>
-      <c r="V18" s="4" t="s">
+      <c r="W18" s="2">
+        <v>2</v>
+      </c>
+      <c r="X18" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="W18" s="4" t="s">
+      <c r="Y18" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="X18" s="4" t="s">
+      <c r="Z18" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y18" s="4" t="s">
+      <c r="AA18" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="Z18" s="4"/>
-      <c r="AA18" s="4"/>
-      <c r="AB18" s="2" t="s">
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="AC18" s="2" t="s">
+      <c r="AE18" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="AD18" s="2" t="s">
+      <c r="AF18" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="AE18" s="2">
+      <c r="AG18" s="2">
         <v>123</v>
       </c>
-      <c r="AF18" s="2">
+      <c r="AH18" s="2">
         <v>2908</v>
       </c>
-      <c r="AG18" s="2">
+      <c r="AI18" s="2">
         <v>2003</v>
       </c>
-      <c r="AH18" s="4" t="s">
+      <c r="AJ18" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="AI18" s="4" t="s">
+      <c r="AK18" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="AJ18" s="2" t="s">
+      <c r="AL18" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="AK18" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL18" s="2">
-        <v>1</v>
-      </c>
       <c r="AM18" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN18" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO18" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H19" s="2">
-        <v>1</v>
-      </c>
       <c r="I19" s="2">
         <v>1</v>
       </c>
@@ -3737,108 +3817,112 @@
         <v>1</v>
       </c>
       <c r="M19" s="2">
+        <v>1</v>
+      </c>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2">
         <v>35</v>
       </c>
-      <c r="N19" s="2">
-        <v>1</v>
-      </c>
-      <c r="O19" s="2">
-        <v>2</v>
-      </c>
-      <c r="P19" s="6" t="s">
+      <c r="P19" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>2</v>
+      </c>
+      <c r="R19" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="Q19" s="6" t="s">
+      <c r="S19" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="R19" s="2" t="s">
+      <c r="T19" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="S19" s="2" t="s">
+      <c r="U19" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="T19" s="2">
+      <c r="V19" s="2">
         <v>98</v>
       </c>
-      <c r="U19" s="2">
-        <v>2</v>
-      </c>
-      <c r="V19" s="4" t="s">
+      <c r="W19" s="2">
+        <v>2</v>
+      </c>
+      <c r="X19" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="W19" s="4" t="s">
+      <c r="Y19" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="X19" s="4" t="s">
+      <c r="Z19" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y19" s="4" t="s">
+      <c r="AA19" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="Z19" s="4"/>
-      <c r="AA19" s="4"/>
-      <c r="AB19" s="2" t="s">
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="AC19" s="2" t="s">
+      <c r="AE19" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="AD19" s="2" t="s">
+      <c r="AF19" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="AE19" s="2">
+      <c r="AG19" s="2">
         <v>123</v>
       </c>
-      <c r="AF19" s="2">
+      <c r="AH19" s="2">
         <v>2908</v>
       </c>
-      <c r="AG19" s="2">
+      <c r="AI19" s="2">
         <v>2003</v>
       </c>
-      <c r="AH19" s="4" t="s">
+      <c r="AJ19" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="AI19" s="4" t="s">
+      <c r="AK19" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="AJ19" s="2" t="s">
+      <c r="AL19" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="AK19" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL19" s="2">
-        <v>1</v>
-      </c>
       <c r="AM19" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN19" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO19" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="H20" s="2">
-        <v>1</v>
-      </c>
       <c r="I20" s="2">
         <v>1</v>
       </c>
@@ -3852,108 +3936,112 @@
         <v>1</v>
       </c>
       <c r="M20" s="2">
+        <v>1</v>
+      </c>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2">
         <v>37</v>
       </c>
-      <c r="N20" s="2">
-        <v>1</v>
-      </c>
-      <c r="O20" s="2">
-        <v>2</v>
-      </c>
-      <c r="P20" s="6" t="s">
+      <c r="P20" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>2</v>
+      </c>
+      <c r="R20" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="Q20" s="6" t="s">
+      <c r="S20" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="R20" s="2" t="s">
+      <c r="T20" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="S20" s="2" t="s">
+      <c r="U20" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="T20" s="2">
+      <c r="V20" s="2">
         <v>98</v>
       </c>
-      <c r="U20" s="2">
-        <v>2</v>
-      </c>
-      <c r="V20" s="4" t="s">
+      <c r="W20" s="2">
+        <v>2</v>
+      </c>
+      <c r="X20" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="W20" s="4" t="s">
+      <c r="Y20" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="X20" s="4" t="s">
+      <c r="Z20" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y20" s="4" t="s">
+      <c r="AA20" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="Z20" s="4"/>
-      <c r="AA20" s="4"/>
-      <c r="AB20" s="2" t="s">
+      <c r="AB20" s="4"/>
+      <c r="AC20" s="4"/>
+      <c r="AD20" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="AC20" s="2" t="s">
+      <c r="AE20" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="AD20" s="2" t="s">
+      <c r="AF20" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="AE20" s="2">
+      <c r="AG20" s="2">
         <v>123</v>
       </c>
-      <c r="AF20" s="2">
+      <c r="AH20" s="2">
         <v>2908</v>
       </c>
-      <c r="AG20" s="2">
+      <c r="AI20" s="2">
         <v>2003</v>
       </c>
-      <c r="AH20" s="4" t="s">
+      <c r="AJ20" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="AI20" s="4" t="s">
+      <c r="AK20" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="AJ20" s="2" t="s">
+      <c r="AL20" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="AK20" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL20" s="2">
-        <v>1</v>
-      </c>
       <c r="AM20" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN20" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO20" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="H21" s="2">
-        <v>1</v>
-      </c>
       <c r="I21" s="2">
         <v>1</v>
       </c>
@@ -3967,108 +4055,112 @@
         <v>1</v>
       </c>
       <c r="M21" s="2">
+        <v>1</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2">
         <v>39</v>
       </c>
-      <c r="N21" s="2">
-        <v>1</v>
-      </c>
-      <c r="O21" s="2">
-        <v>2</v>
-      </c>
-      <c r="P21" s="6" t="s">
+      <c r="P21" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>2</v>
+      </c>
+      <c r="R21" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="Q21" s="6" t="s">
+      <c r="S21" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="R21" s="2" t="s">
+      <c r="T21" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="S21" s="2" t="s">
+      <c r="U21" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="T21" s="2">
+      <c r="V21" s="2">
         <v>98</v>
       </c>
-      <c r="U21" s="2">
-        <v>2</v>
-      </c>
-      <c r="V21" s="4" t="s">
+      <c r="W21" s="2">
+        <v>2</v>
+      </c>
+      <c r="X21" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="W21" s="4" t="s">
+      <c r="Y21" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="X21" s="4" t="s">
+      <c r="Z21" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y21" s="4" t="s">
+      <c r="AA21" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="Z21" s="4"/>
-      <c r="AA21" s="4"/>
-      <c r="AB21" s="2" t="s">
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="AC21" s="2" t="s">
+      <c r="AE21" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="AD21" s="2" t="s">
+      <c r="AF21" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="AE21" s="2">
+      <c r="AG21" s="2">
         <v>123</v>
       </c>
-      <c r="AF21" s="2">
+      <c r="AH21" s="2">
         <v>2908</v>
       </c>
-      <c r="AG21" s="2">
+      <c r="AI21" s="2">
         <v>2003</v>
       </c>
-      <c r="AH21" s="4" t="s">
+      <c r="AJ21" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="AI21" s="4" t="s">
+      <c r="AK21" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="AJ21" s="2" t="s">
+      <c r="AL21" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="AK21" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL21" s="2">
-        <v>1</v>
-      </c>
       <c r="AM21" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN21" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO21" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>3</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="H22" s="2">
-        <v>1</v>
-      </c>
       <c r="I22" s="2">
         <v>1</v>
       </c>
@@ -4082,96 +4174,100 @@
         <v>1</v>
       </c>
       <c r="M22" s="2">
+        <v>1</v>
+      </c>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2">
         <v>41</v>
       </c>
-      <c r="N22" s="2">
-        <v>1</v>
-      </c>
-      <c r="O22" s="2">
-        <v>1</v>
-      </c>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
+      <c r="P22" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>1</v>
+      </c>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
-      <c r="V22" s="4" t="s">
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="W22" s="4" t="s">
+      <c r="Y22" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="X22" s="4" t="s">
+      <c r="Z22" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y22" s="4" t="s">
+      <c r="AA22" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="Z22" s="4"/>
-      <c r="AA22" s="4"/>
-      <c r="AB22" s="2" t="s">
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="4"/>
+      <c r="AD22" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AC22" s="2" t="s">
+      <c r="AE22" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="AD22" s="2" t="s">
+      <c r="AF22" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="AE22" s="2">
+      <c r="AG22" s="2">
         <v>123</v>
       </c>
-      <c r="AF22" s="2">
+      <c r="AH22" s="2">
         <v>2908</v>
       </c>
-      <c r="AG22" s="2">
+      <c r="AI22" s="2">
         <v>2003</v>
       </c>
-      <c r="AH22" s="4" t="s">
+      <c r="AJ22" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="AI22" s="4" t="s">
+      <c r="AK22" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="AJ22" s="2" t="s">
+      <c r="AL22" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="AK22" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL22" s="2">
-        <v>1</v>
-      </c>
       <c r="AM22" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN22" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO22" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="H23" s="2">
-        <v>1</v>
-      </c>
       <c r="I23" s="2">
         <v>1</v>
       </c>
@@ -4185,96 +4281,100 @@
         <v>1</v>
       </c>
       <c r="M23" s="2">
+        <v>1</v>
+      </c>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2">
         <v>43</v>
       </c>
-      <c r="N23" s="2">
-        <v>1</v>
-      </c>
-      <c r="O23" s="2">
-        <v>1</v>
-      </c>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
+      <c r="P23" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>1</v>
+      </c>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
-      <c r="V23" s="4" t="s">
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="W23" s="4" t="s">
+      <c r="Y23" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="X23" s="4" t="s">
+      <c r="Z23" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y23" s="4" t="s">
+      <c r="AA23" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="Z23" s="4"/>
-      <c r="AA23" s="4"/>
-      <c r="AB23" s="2" t="s">
+      <c r="AB23" s="4"/>
+      <c r="AC23" s="4"/>
+      <c r="AD23" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="AC23" s="2" t="s">
+      <c r="AE23" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="AD23" s="2" t="s">
+      <c r="AF23" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="AE23" s="2">
+      <c r="AG23" s="2">
         <v>123</v>
       </c>
-      <c r="AF23" s="2">
+      <c r="AH23" s="2">
         <v>2908</v>
       </c>
-      <c r="AG23" s="2">
+      <c r="AI23" s="2">
         <v>2003</v>
       </c>
-      <c r="AH23" s="4" t="s">
+      <c r="AJ23" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="AI23" s="4" t="s">
+      <c r="AK23" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="AJ23" s="2" t="s">
+      <c r="AL23" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="AK23" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL23" s="2">
-        <v>1</v>
-      </c>
       <c r="AM23" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN23" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO23" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="H24" s="2">
-        <v>1</v>
-      </c>
       <c r="I24" s="2">
         <v>1</v>
       </c>
@@ -4288,96 +4388,100 @@
         <v>1</v>
       </c>
       <c r="M24" s="2">
+        <v>1</v>
+      </c>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2">
         <v>45</v>
       </c>
-      <c r="N24" s="2">
-        <v>1</v>
-      </c>
-      <c r="O24" s="2">
-        <v>1</v>
-      </c>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
+      <c r="P24" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>1</v>
+      </c>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
-      <c r="V24" s="4" t="s">
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="W24" s="4" t="s">
+      <c r="Y24" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="X24" s="4" t="s">
+      <c r="Z24" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="Y24" s="4" t="s">
+      <c r="AA24" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="Z24" s="4"/>
-      <c r="AA24" s="4"/>
-      <c r="AB24" s="2" t="s">
+      <c r="AB24" s="4"/>
+      <c r="AC24" s="4"/>
+      <c r="AD24" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="AC24" s="2" t="s">
+      <c r="AE24" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="AD24" s="2" t="s">
+      <c r="AF24" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="AE24" s="2">
+      <c r="AG24" s="2">
         <v>123</v>
       </c>
-      <c r="AF24" s="2">
+      <c r="AH24" s="2">
         <v>2908</v>
       </c>
-      <c r="AG24" s="2">
+      <c r="AI24" s="2">
         <v>2003</v>
       </c>
-      <c r="AH24" s="4" t="s">
+      <c r="AJ24" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="AI24" s="4" t="s">
+      <c r="AK24" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="AJ24" s="2" t="s">
+      <c r="AL24" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="AK24" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL24" s="2">
-        <v>1</v>
-      </c>
       <c r="AM24" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN24" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO24" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>3</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="H25" s="2">
-        <v>1</v>
-      </c>
       <c r="I25" s="2">
         <v>1</v>
       </c>
@@ -4385,96 +4489,102 @@
         <v>1</v>
       </c>
       <c r="K25" s="2">
+        <v>1</v>
+      </c>
+      <c r="L25" s="2">
         <v>3</v>
       </c>
-      <c r="L25" s="2">
-        <v>2</v>
-      </c>
-      <c r="M25" s="2"/>
+      <c r="M25" s="2">
+        <v>2</v>
+      </c>
       <c r="N25" s="2">
-        <v>1</v>
-      </c>
-      <c r="O25" s="2">
-        <v>1</v>
-      </c>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>1</v>
+      </c>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
-      <c r="V25" s="4" t="s">
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="W25" s="4" t="s">
+      <c r="Y25" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
       <c r="Z25" s="4"/>
       <c r="AA25" s="4"/>
-      <c r="AB25" s="2" t="s">
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="4"/>
+      <c r="AD25" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="AC25" s="2" t="s">
+      <c r="AE25" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="AD25" s="2" t="s">
+      <c r="AF25" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="AE25" s="2">
+      <c r="AG25" s="2">
         <v>123</v>
       </c>
-      <c r="AF25" s="2">
+      <c r="AH25" s="2">
         <v>2908</v>
       </c>
-      <c r="AG25" s="2">
+      <c r="AI25" s="2">
         <v>2003</v>
       </c>
-      <c r="AH25" s="4" t="s">
+      <c r="AJ25" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="AI25" s="4" t="s">
+      <c r="AK25" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="AJ25" s="2" t="s">
+      <c r="AL25" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="AK25" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL25" s="2">
-        <v>1</v>
-      </c>
       <c r="AM25" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN25" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO25" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>3</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="H26" s="2">
-        <v>1</v>
-      </c>
       <c r="I26" s="2">
         <v>1</v>
       </c>
@@ -4482,96 +4592,102 @@
         <v>1</v>
       </c>
       <c r="K26" s="2">
+        <v>1</v>
+      </c>
+      <c r="L26" s="2">
         <v>3</v>
       </c>
-      <c r="L26" s="2">
-        <v>2</v>
-      </c>
-      <c r="M26" s="2"/>
+      <c r="M26" s="2">
+        <v>2</v>
+      </c>
       <c r="N26" s="2">
-        <v>1</v>
-      </c>
-      <c r="O26" s="2">
-        <v>1</v>
-      </c>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>1</v>
+      </c>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
-      <c r="V26" s="4" t="s">
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="W26" s="4" t="s">
+      <c r="Y26" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
       <c r="Z26" s="4"/>
       <c r="AA26" s="4"/>
-      <c r="AB26" s="2" t="s">
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="4"/>
+      <c r="AD26" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AC26" s="2" t="s">
+      <c r="AE26" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="AD26" s="2" t="s">
+      <c r="AF26" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="AE26" s="2">
+      <c r="AG26" s="2">
         <v>123</v>
       </c>
-      <c r="AF26" s="2">
+      <c r="AH26" s="2">
         <v>2908</v>
       </c>
-      <c r="AG26" s="2">
+      <c r="AI26" s="2">
         <v>2003</v>
       </c>
-      <c r="AH26" s="4" t="s">
+      <c r="AJ26" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="AI26" s="4" t="s">
+      <c r="AK26" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="AJ26" s="2" t="s">
+      <c r="AL26" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="AK26" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL26" s="2">
-        <v>1</v>
-      </c>
       <c r="AM26" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN26" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO26" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>3</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="G27" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="H27" s="2">
-        <v>1</v>
-      </c>
       <c r="I27" s="2">
         <v>1</v>
       </c>
@@ -4579,96 +4695,102 @@
         <v>1</v>
       </c>
       <c r="K27" s="2">
+        <v>1</v>
+      </c>
+      <c r="L27" s="2">
         <v>3</v>
       </c>
-      <c r="L27" s="2">
-        <v>2</v>
-      </c>
-      <c r="M27" s="2"/>
+      <c r="M27" s="2">
+        <v>2</v>
+      </c>
       <c r="N27" s="2">
-        <v>1</v>
-      </c>
-      <c r="O27" s="2">
-        <v>1</v>
-      </c>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>1</v>
+      </c>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
-      <c r="V27" s="4" t="s">
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="W27" s="4" t="s">
+      <c r="Y27" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
       <c r="Z27" s="4"/>
       <c r="AA27" s="4"/>
-      <c r="AB27" s="2" t="s">
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="4"/>
+      <c r="AD27" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="AC27" s="2" t="s">
+      <c r="AE27" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="AD27" s="2" t="s">
+      <c r="AF27" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AE27" s="2">
+      <c r="AG27" s="2">
         <v>123</v>
       </c>
-      <c r="AF27" s="2">
+      <c r="AH27" s="2">
         <v>2908</v>
       </c>
-      <c r="AG27" s="2">
+      <c r="AI27" s="2">
         <v>2003</v>
       </c>
-      <c r="AH27" s="4" t="s">
+      <c r="AJ27" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="AI27" s="4" t="s">
+      <c r="AK27" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="AJ27" s="2" t="s">
+      <c r="AL27" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="AK27" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL27" s="2">
-        <v>1</v>
-      </c>
       <c r="AM27" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN27" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO27" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>3</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="G28" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="H28" s="2">
-        <v>1</v>
-      </c>
       <c r="I28" s="2">
         <v>1</v>
       </c>
@@ -4676,73 +4798,79 @@
         <v>1</v>
       </c>
       <c r="K28" s="2">
+        <v>1</v>
+      </c>
+      <c r="L28" s="2">
         <v>3</v>
       </c>
-      <c r="L28" s="2">
-        <v>2</v>
-      </c>
-      <c r="M28" s="2"/>
+      <c r="M28" s="2">
+        <v>2</v>
+      </c>
       <c r="N28" s="2">
         <v>1</v>
       </c>
-      <c r="O28" s="2">
-        <v>1</v>
-      </c>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>1</v>
+      </c>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
-      <c r="V28" s="4" t="s">
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="W28" s="4" t="s">
+      <c r="Y28" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
       <c r="Z28" s="4"/>
       <c r="AA28" s="4"/>
-      <c r="AB28" s="2" t="s">
+      <c r="AB28" s="4"/>
+      <c r="AC28" s="4"/>
+      <c r="AD28" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AC28" s="2" t="s">
+      <c r="AE28" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="AD28" s="2" t="s">
+      <c r="AF28" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="AE28" s="2">
+      <c r="AG28" s="2">
         <v>123</v>
       </c>
-      <c r="AF28" s="2">
+      <c r="AH28" s="2">
         <v>2908</v>
       </c>
-      <c r="AG28" s="2">
+      <c r="AI28" s="2">
         <v>2003</v>
       </c>
-      <c r="AH28" s="4" t="s">
+      <c r="AJ28" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="AI28" s="4" t="s">
+      <c r="AK28" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="AJ28" s="2" t="s">
+      <c r="AL28" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="AK28" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL28" s="2">
-        <v>1</v>
-      </c>
       <c r="AM28" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN28" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO28" s="2">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM28"/>
+  <autoFilter ref="B1:AO28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
from house 24/02/2025 at 01:12
</commit_message>
<xml_diff>
--- a/app/Imports/data-excel-2025.xlsx
+++ b/app/Imports/data-excel-2025.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\projects\grace-app\back_grace\app\Imports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Grace Project\grace_back\app\Imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6571177-81FE-4267-9955-5B8907859D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10830"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -659,9 +660,6 @@
     <t>cin27</t>
   </si>
   <si>
-    <t>1009/2051</t>
-  </si>
-  <si>
     <t>1988-09-11</t>
   </si>
   <si>
@@ -1410,12 +1408,15 @@
   </si>
   <si>
     <t>user_id</t>
+  </si>
+  <si>
+    <t>1009/2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1767,10 +1768,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1805,7 +1808,7 @@
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1838,40 +1841,40 @@
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>310</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>313</v>
-      </c>
       <c r="U1" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>332</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>333</v>
       </c>
       <c r="X1" s="3" t="s">
         <v>11</v>
@@ -1880,25 +1883,25 @@
         <v>12</v>
       </c>
       <c r="Z1" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="AA1" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="AA1" s="3" t="s">
-        <v>335</v>
-      </c>
       <c r="AB1" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC1" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>341</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>14</v>
@@ -1910,7 +1913,7 @@
         <v>16</v>
       </c>
       <c r="AJ1" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AK1" s="3" t="s">
         <v>17</v>
@@ -1948,7 +1951,7 @@
         <v>74</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>75</v>
@@ -1985,16 +1988,16 @@
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Z2" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="AA2" s="4" t="s">
         <v>336</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>337</v>
       </c>
       <c r="AB2" s="4"/>
       <c r="AC2" s="4"/>
@@ -2002,10 +2005,10 @@
         <v>76</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AG2" s="2">
         <v>123</v>
@@ -2017,13 +2020,13 @@
         <v>2003</v>
       </c>
       <c r="AJ2" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AK2" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AL2" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AM2" s="2">
         <v>1</v>
@@ -2055,7 +2058,7 @@
         <v>105</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>106</v>
@@ -2092,16 +2095,16 @@
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Z3" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="AA3" s="4" t="s">
         <v>336</v>
-      </c>
-      <c r="AA3" s="4" t="s">
-        <v>337</v>
       </c>
       <c r="AB3" s="4"/>
       <c r="AC3" s="4"/>
@@ -2109,10 +2112,10 @@
         <v>77</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AG3" s="2">
         <v>123</v>
@@ -2124,13 +2127,13 @@
         <v>2003</v>
       </c>
       <c r="AJ3" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AK3" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AL3" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AM3" s="2">
         <v>1</v>
@@ -2162,7 +2165,7 @@
         <v>109</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>110</v>
@@ -2199,10 +2202,10 @@
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
       <c r="X4" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
@@ -2212,10 +2215,10 @@
         <v>78</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AG4" s="2">
         <v>123</v>
@@ -2227,13 +2230,13 @@
         <v>2003</v>
       </c>
       <c r="AJ4" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AK4" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AL4" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="AM4" s="2">
         <v>1</v>
@@ -2265,7 +2268,7 @@
         <v>113</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>114</v>
@@ -2302,16 +2305,16 @@
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
       <c r="X5" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Z5" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="AA5" s="4" t="s">
         <v>336</v>
-      </c>
-      <c r="AA5" s="4" t="s">
-        <v>337</v>
       </c>
       <c r="AB5" s="4"/>
       <c r="AC5" s="4"/>
@@ -2319,10 +2322,10 @@
         <v>79</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AG5" s="2">
         <v>123</v>
@@ -2334,13 +2337,13 @@
         <v>2003</v>
       </c>
       <c r="AJ5" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AK5" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AL5" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AM5" s="2">
         <v>1</v>
@@ -2372,7 +2375,7 @@
         <v>117</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>118</v>
@@ -2409,16 +2412,16 @@
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
       <c r="X6" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Z6" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="AA6" s="4" t="s">
         <v>336</v>
-      </c>
-      <c r="AA6" s="4" t="s">
-        <v>337</v>
       </c>
       <c r="AB6" s="4"/>
       <c r="AC6" s="4"/>
@@ -2426,10 +2429,10 @@
         <v>80</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AG6" s="2">
         <v>123</v>
@@ -2441,13 +2444,13 @@
         <v>2003</v>
       </c>
       <c r="AJ6" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AK6" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AL6" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AM6" s="2">
         <v>1</v>
@@ -2479,7 +2482,7 @@
         <v>121</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>122</v>
@@ -2516,16 +2519,16 @@
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
       <c r="X7" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Z7" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="AA7" s="4" t="s">
         <v>336</v>
-      </c>
-      <c r="AA7" s="4" t="s">
-        <v>337</v>
       </c>
       <c r="AB7" s="4"/>
       <c r="AC7" s="4"/>
@@ -2533,10 +2536,10 @@
         <v>81</v>
       </c>
       <c r="AE7" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="AF7" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AG7" s="2">
         <v>123</v>
@@ -2548,13 +2551,13 @@
         <v>2003</v>
       </c>
       <c r="AJ7" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AK7" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AL7" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AM7" s="2">
         <v>1</v>
@@ -2586,7 +2589,7 @@
         <v>125</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>126</v>
@@ -2623,16 +2626,16 @@
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
       <c r="X8" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Z8" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="AA8" s="4" t="s">
         <v>336</v>
-      </c>
-      <c r="AA8" s="4" t="s">
-        <v>337</v>
       </c>
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
@@ -2640,10 +2643,10 @@
         <v>82</v>
       </c>
       <c r="AE8" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AF8" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AG8" s="2">
         <v>123</v>
@@ -2655,13 +2658,13 @@
         <v>2003</v>
       </c>
       <c r="AJ8" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AK8" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AL8" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AM8" s="2">
         <v>1</v>
@@ -2693,7 +2696,7 @@
         <v>129</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>130</v>
@@ -2730,16 +2733,16 @@
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
       <c r="X9" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Z9" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="AA9" s="4" t="s">
         <v>336</v>
-      </c>
-      <c r="AA9" s="4" t="s">
-        <v>337</v>
       </c>
       <c r="AB9" s="4"/>
       <c r="AC9" s="4"/>
@@ -2747,10 +2750,10 @@
         <v>83</v>
       </c>
       <c r="AE9" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AF9" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AG9" s="2">
         <v>123</v>
@@ -2762,13 +2765,13 @@
         <v>2003</v>
       </c>
       <c r="AJ9" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AK9" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AL9" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="AM9" s="2">
         <v>1</v>
@@ -2800,7 +2803,7 @@
         <v>133</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>134</v>
@@ -2837,16 +2840,16 @@
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
       <c r="X10" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Z10" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="AA10" s="4" t="s">
         <v>336</v>
-      </c>
-      <c r="AA10" s="4" t="s">
-        <v>337</v>
       </c>
       <c r="AB10" s="4"/>
       <c r="AC10" s="4"/>
@@ -2854,10 +2857,10 @@
         <v>84</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AG10" s="2">
         <v>123</v>
@@ -2869,13 +2872,13 @@
         <v>2003</v>
       </c>
       <c r="AJ10" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AK10" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AL10" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AM10" s="2">
         <v>1</v>
@@ -2907,7 +2910,7 @@
         <v>137</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>138</v>
@@ -2944,16 +2947,16 @@
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
       <c r="X11" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Y11" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Z11" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AA11" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AB11" s="4"/>
       <c r="AC11" s="4"/>
@@ -2961,10 +2964,10 @@
         <v>85</v>
       </c>
       <c r="AE11" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AF11" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AG11" s="2">
         <v>123</v>
@@ -2976,13 +2979,13 @@
         <v>2003</v>
       </c>
       <c r="AJ11" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AK11" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AL11" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AM11" s="2">
         <v>1</v>
@@ -3014,7 +3017,7 @@
         <v>141</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>142</v>
@@ -3051,16 +3054,16 @@
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
       <c r="X12" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Z12" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AA12" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AB12" s="4"/>
       <c r="AC12" s="4"/>
@@ -3068,10 +3071,10 @@
         <v>86</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="AF12" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AG12" s="2">
         <v>123</v>
@@ -3083,13 +3086,13 @@
         <v>2003</v>
       </c>
       <c r="AJ12" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AK12" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="AL12" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AM12" s="2">
         <v>1</v>
@@ -3121,7 +3124,7 @@
         <v>145</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>146</v>
@@ -3158,16 +3161,16 @@
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
       <c r="X13" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y13" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Z13" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AA13" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AB13" s="4"/>
       <c r="AC13" s="4"/>
@@ -3175,10 +3178,10 @@
         <v>87</v>
       </c>
       <c r="AE13" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="AF13" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AG13" s="2">
         <v>123</v>
@@ -3190,13 +3193,13 @@
         <v>2003</v>
       </c>
       <c r="AJ13" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AK13" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AL13" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AM13" s="2">
         <v>1</v>
@@ -3228,7 +3231,7 @@
         <v>149</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>150</v>
@@ -3265,16 +3268,16 @@
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
       <c r="X14" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Y14" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Z14" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AA14" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AB14" s="4"/>
       <c r="AC14" s="4"/>
@@ -3282,10 +3285,10 @@
         <v>88</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="AG14" s="2">
         <v>123</v>
@@ -3297,13 +3300,13 @@
         <v>2003</v>
       </c>
       <c r="AJ14" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AK14" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AL14" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AM14" s="2">
         <v>1</v>
@@ -3335,7 +3338,7 @@
         <v>153</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>154</v>
@@ -3372,16 +3375,16 @@
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
       <c r="X15" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Y15" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Z15" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AA15" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AB15" s="4"/>
       <c r="AC15" s="4"/>
@@ -3389,10 +3392,10 @@
         <v>89</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AF15" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AG15" s="2">
         <v>123</v>
@@ -3404,13 +3407,13 @@
         <v>2003</v>
       </c>
       <c r="AJ15" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AK15" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AL15" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="AM15" s="2">
         <v>1</v>
@@ -3442,7 +3445,7 @@
         <v>157</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>158</v>
@@ -3473,16 +3476,16 @@
         <v>2</v>
       </c>
       <c r="R16" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="S16" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="V16" s="2">
         <v>98</v>
@@ -3491,16 +3494,16 @@
         <v>2</v>
       </c>
       <c r="X16" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Y16" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Z16" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AA16" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AB16" s="4"/>
       <c r="AC16" s="4"/>
@@ -3508,10 +3511,10 @@
         <v>90</v>
       </c>
       <c r="AE16" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AF16" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AG16" s="2">
         <v>123</v>
@@ -3523,13 +3526,13 @@
         <v>2003</v>
       </c>
       <c r="AJ16" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AK16" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AL16" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="AM16" s="2">
         <v>1</v>
@@ -3561,7 +3564,7 @@
         <v>161</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>162</v>
@@ -3592,16 +3595,16 @@
         <v>2</v>
       </c>
       <c r="R17" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="S17" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="V17" s="2">
         <v>98</v>
@@ -3610,16 +3613,16 @@
         <v>2</v>
       </c>
       <c r="X17" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Y17" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Z17" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AA17" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AB17" s="4"/>
       <c r="AC17" s="4"/>
@@ -3627,10 +3630,10 @@
         <v>91</v>
       </c>
       <c r="AE17" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="AF17" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AG17" s="2">
         <v>123</v>
@@ -3642,13 +3645,13 @@
         <v>2003</v>
       </c>
       <c r="AJ17" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AK17" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AL17" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AM17" s="2">
         <v>1</v>
@@ -3680,7 +3683,7 @@
         <v>165</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>166</v>
@@ -3711,16 +3714,16 @@
         <v>2</v>
       </c>
       <c r="R18" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S18" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="V18" s="2">
         <v>98</v>
@@ -3729,16 +3732,16 @@
         <v>2</v>
       </c>
       <c r="X18" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Y18" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Z18" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AA18" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AB18" s="4"/>
       <c r="AC18" s="4"/>
@@ -3746,10 +3749,10 @@
         <v>92</v>
       </c>
       <c r="AE18" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="AF18" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AG18" s="2">
         <v>123</v>
@@ -3761,13 +3764,13 @@
         <v>2003</v>
       </c>
       <c r="AJ18" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AK18" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AL18" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AM18" s="2">
         <v>1</v>
@@ -3799,7 +3802,7 @@
         <v>169</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>170</v>
@@ -3830,16 +3833,16 @@
         <v>2</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="S19" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="V19" s="2">
         <v>98</v>
@@ -3848,16 +3851,16 @@
         <v>2</v>
       </c>
       <c r="X19" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Y19" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Z19" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AA19" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
@@ -3865,10 +3868,10 @@
         <v>93</v>
       </c>
       <c r="AE19" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="AF19" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AG19" s="2">
         <v>123</v>
@@ -3880,13 +3883,13 @@
         <v>2003</v>
       </c>
       <c r="AJ19" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AK19" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AL19" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AM19" s="2">
         <v>1</v>
@@ -3918,7 +3921,7 @@
         <v>173</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>174</v>
@@ -3949,16 +3952,16 @@
         <v>2</v>
       </c>
       <c r="R20" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="S20" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="V20" s="2">
         <v>98</v>
@@ -3967,16 +3970,16 @@
         <v>2</v>
       </c>
       <c r="X20" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Y20" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Z20" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AA20" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AB20" s="4"/>
       <c r="AC20" s="4"/>
@@ -3984,10 +3987,10 @@
         <v>94</v>
       </c>
       <c r="AE20" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="AF20" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AG20" s="2">
         <v>123</v>
@@ -3999,13 +4002,13 @@
         <v>2003</v>
       </c>
       <c r="AJ20" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AK20" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AL20" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AM20" s="2">
         <v>1</v>
@@ -4037,7 +4040,7 @@
         <v>177</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>178</v>
@@ -4068,16 +4071,16 @@
         <v>2</v>
       </c>
       <c r="R21" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="S21" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="V21" s="2">
         <v>98</v>
@@ -4086,16 +4089,16 @@
         <v>2</v>
       </c>
       <c r="X21" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Y21" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Z21" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AA21" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
@@ -4103,10 +4106,10 @@
         <v>95</v>
       </c>
       <c r="AE21" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AF21" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AG21" s="2">
         <v>123</v>
@@ -4118,13 +4121,13 @@
         <v>2003</v>
       </c>
       <c r="AJ21" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AK21" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AL21" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="AM21" s="2">
         <v>1</v>
@@ -4156,7 +4159,7 @@
         <v>181</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>182</v>
@@ -4193,16 +4196,16 @@
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
       <c r="X22" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Y22" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Z22" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AA22" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
@@ -4210,10 +4213,10 @@
         <v>96</v>
       </c>
       <c r="AE22" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AF22" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AG22" s="2">
         <v>123</v>
@@ -4225,13 +4228,13 @@
         <v>2003</v>
       </c>
       <c r="AJ22" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AK22" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AL22" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="AM22" s="2">
         <v>1</v>
@@ -4263,7 +4266,7 @@
         <v>185</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>186</v>
@@ -4300,16 +4303,16 @@
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
       <c r="X23" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y23" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Z23" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AA23" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AB23" s="4"/>
       <c r="AC23" s="4"/>
@@ -4317,10 +4320,10 @@
         <v>97</v>
       </c>
       <c r="AE23" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="AF23" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AG23" s="2">
         <v>123</v>
@@ -4332,13 +4335,13 @@
         <v>2003</v>
       </c>
       <c r="AJ23" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AK23" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AL23" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="AM23" s="2">
         <v>1</v>
@@ -4370,7 +4373,7 @@
         <v>189</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>190</v>
@@ -4407,16 +4410,16 @@
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
       <c r="X24" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Y24" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Z24" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AA24" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
@@ -4424,10 +4427,10 @@
         <v>98</v>
       </c>
       <c r="AE24" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="AF24" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AG24" s="2">
         <v>123</v>
@@ -4439,13 +4442,13 @@
         <v>2003</v>
       </c>
       <c r="AJ24" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AK24" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AL24" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="AM24" s="2">
         <v>1</v>
@@ -4477,7 +4480,7 @@
         <v>194</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>195</v>
@@ -4514,10 +4517,10 @@
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
       <c r="X25" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Y25" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Z25" s="4"/>
       <c r="AA25" s="4"/>
@@ -4527,10 +4530,10 @@
         <v>99</v>
       </c>
       <c r="AE25" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="AF25" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AG25" s="2">
         <v>123</v>
@@ -4542,13 +4545,13 @@
         <v>2003</v>
       </c>
       <c r="AJ25" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AK25" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AL25" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="AM25" s="2">
         <v>1</v>
@@ -4580,7 +4583,7 @@
         <v>199</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>200</v>
@@ -4617,10 +4620,10 @@
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
       <c r="X26" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Y26" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Z26" s="4"/>
       <c r="AA26" s="4"/>
@@ -4630,10 +4633,10 @@
         <v>100</v>
       </c>
       <c r="AE26" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AF26" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AG26" s="2">
         <v>123</v>
@@ -4645,13 +4648,13 @@
         <v>2003</v>
       </c>
       <c r="AJ26" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AK26" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AL26" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AM26" s="2">
         <v>1</v>
@@ -4683,7 +4686,7 @@
         <v>204</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>205</v>
@@ -4720,10 +4723,10 @@
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
       <c r="X27" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Y27" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Z27" s="4"/>
       <c r="AA27" s="4"/>
@@ -4733,10 +4736,10 @@
         <v>101</v>
       </c>
       <c r="AE27" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="AF27" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AG27" s="2">
         <v>123</v>
@@ -4748,13 +4751,13 @@
         <v>2003</v>
       </c>
       <c r="AJ27" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AK27" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AL27" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="AM27" s="2">
         <v>1</v>
@@ -4786,10 +4789,10 @@
         <v>209</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>210</v>
+        <v>460</v>
       </c>
       <c r="I28" s="2">
         <v>1</v>
@@ -4823,10 +4826,10 @@
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
       <c r="X28" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Y28" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Z28" s="4"/>
       <c r="AA28" s="4"/>
@@ -4836,10 +4839,10 @@
         <v>102</v>
       </c>
       <c r="AE28" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AF28" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AG28" s="2">
         <v>123</v>
@@ -4851,13 +4854,13 @@
         <v>2003</v>
       </c>
       <c r="AJ28" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AK28" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AL28" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AM28" s="2">
         <v>1</v>
@@ -4870,7 +4873,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:AO28"/>
+  <autoFilter ref="B1:AO28" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
from work 26/02/2025 at 16h16
</commit_message>
<xml_diff>
--- a/app/Imports/data-excel-2025.xlsx
+++ b/app/Imports/data-excel-2025.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Grace Project\grace_back\app\Imports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\grace_back\app\Imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6571177-81FE-4267-9955-5B8907859D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1416,7 +1415,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1768,11 +1767,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4873,7 +4872,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:AO28" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B1:AO28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
09/05/2025 at 16h15 working
</commit_message>
<xml_diff>
--- a/app/Imports/data-excel-2025.xlsx
+++ b/app/Imports/data-excel-2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\grace_back\app\Imports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.benaya\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$1:$AH$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$1:$AI$28</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="469">
   <si>
     <t>nom</t>
   </si>
@@ -1422,6 +1422,18 @@
   </si>
   <si>
     <t>ملاحظة</t>
+  </si>
+  <si>
+    <t>tribunalaffaire</t>
+  </si>
+  <si>
+    <t>92:92:92</t>
+  </si>
+  <si>
+    <t>98:98:98</t>
+  </si>
+  <si>
+    <t>106:106:106</t>
   </si>
 </sst>
 </file>
@@ -1780,10 +1792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS28"/>
+  <dimension ref="A1:AT28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,24 +1816,25 @@
     <col min="21" max="21" width="13.5703125" style="5" customWidth="1"/>
     <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="10.85546875" customWidth="1"/>
-    <col min="25" max="25" width="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.42578125" customWidth="1"/>
-    <col min="29" max="29" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.28515625" customWidth="1"/>
-    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="43" width="14.140625" customWidth="1"/>
-    <col min="44" max="45" width="13.5703125" style="5" customWidth="1"/>
+    <col min="25" max="25" width="25.7109375" customWidth="1"/>
+    <col min="26" max="26" width="8" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.42578125" customWidth="1"/>
+    <col min="30" max="30" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.28515625" customWidth="1"/>
+    <col min="35" max="35" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="44" width="14.140625" customWidth="1"/>
+    <col min="45" max="46" width="13.5703125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>459</v>
       </c>
@@ -1892,71 +1905,74 @@
         <v>429</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>3</v>
       </c>
@@ -2025,38 +2041,38 @@
         <v>430</v>
       </c>
       <c r="X2" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Z2" s="2">
         <v>123</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="AA2" s="2">
         <v>2908</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AB2" s="2">
         <v>2003</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="AE2" s="2">
-        <v>1</v>
-      </c>
       <c r="AF2" s="2">
         <v>1</v>
       </c>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="2"/>
       <c r="AI2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ2" s="2">
         <v>1</v>
@@ -2064,16 +2080,19 @@
       <c r="AK2" s="2">
         <v>1</v>
       </c>
-      <c r="AL2" s="2"/>
+      <c r="AL2" s="2">
+        <v>1</v>
+      </c>
       <c r="AM2" s="2"/>
       <c r="AN2" s="2"/>
       <c r="AO2" s="2"/>
       <c r="AP2" s="2"/>
       <c r="AQ2" s="2"/>
-      <c r="AR2" s="4"/>
+      <c r="AR2" s="2"/>
       <c r="AS2" s="4"/>
+      <c r="AT2" s="4"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>3</v>
       </c>
@@ -2142,38 +2161,38 @@
         <v>431</v>
       </c>
       <c r="X3" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y3" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="Z3" s="2">
         <v>123</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="AA3" s="2">
         <v>2908</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AB3" s="2">
         <v>2003</v>
       </c>
-      <c r="AB3" s="4" t="s">
+      <c r="AC3" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="AC3" s="4" t="s">
+      <c r="AD3" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="AE3" s="2">
-        <v>1</v>
-      </c>
       <c r="AF3" s="2">
         <v>1</v>
       </c>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="2"/>
       <c r="AI3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ3" s="2">
         <v>1</v>
@@ -2181,16 +2200,19 @@
       <c r="AK3" s="2">
         <v>1</v>
       </c>
-      <c r="AL3" s="2"/>
+      <c r="AL3" s="2">
+        <v>1</v>
+      </c>
       <c r="AM3" s="2"/>
       <c r="AN3" s="2"/>
       <c r="AO3" s="2"/>
       <c r="AP3" s="2"/>
       <c r="AQ3" s="2"/>
-      <c r="AR3" s="4"/>
+      <c r="AR3" s="2"/>
       <c r="AS3" s="4"/>
+      <c r="AT3" s="4"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2255,38 +2277,38 @@
         <v>432</v>
       </c>
       <c r="X4" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y4" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="Z4" s="2">
         <v>123</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="AA4" s="2">
         <v>2908</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AB4" s="2">
         <v>2003</v>
       </c>
-      <c r="AB4" s="4" t="s">
+      <c r="AC4" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="AC4" s="4" t="s">
+      <c r="AD4" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="AD4" s="2" t="s">
+      <c r="AE4" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="AE4" s="2">
-        <v>1</v>
-      </c>
       <c r="AF4" s="2">
         <v>1</v>
       </c>
-      <c r="AG4" s="2"/>
-      <c r="AH4" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="2"/>
       <c r="AI4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ4" s="2">
         <v>1</v>
@@ -2294,16 +2316,19 @@
       <c r="AK4" s="2">
         <v>1</v>
       </c>
-      <c r="AL4" s="2"/>
+      <c r="AL4" s="2">
+        <v>1</v>
+      </c>
       <c r="AM4" s="2"/>
       <c r="AN4" s="2"/>
       <c r="AO4" s="2"/>
       <c r="AP4" s="2"/>
       <c r="AQ4" s="2"/>
-      <c r="AR4" s="4"/>
+      <c r="AR4" s="2"/>
       <c r="AS4" s="4"/>
+      <c r="AT4" s="4"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -2372,38 +2397,38 @@
         <v>433</v>
       </c>
       <c r="X5" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y5" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="Z5" s="2">
         <v>123</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="AA5" s="2">
         <v>2908</v>
       </c>
-      <c r="AA5" s="2">
+      <c r="AB5" s="2">
         <v>2003</v>
       </c>
-      <c r="AB5" s="4" t="s">
+      <c r="AC5" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="AC5" s="4" t="s">
+      <c r="AD5" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="AD5" s="2" t="s">
+      <c r="AE5" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="AE5" s="2">
-        <v>1</v>
-      </c>
       <c r="AF5" s="2">
         <v>1</v>
       </c>
-      <c r="AG5" s="2"/>
-      <c r="AH5" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="2"/>
       <c r="AI5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ5" s="2">
         <v>1</v>
@@ -2411,16 +2436,19 @@
       <c r="AK5" s="2">
         <v>1</v>
       </c>
-      <c r="AL5" s="2"/>
+      <c r="AL5" s="2">
+        <v>1</v>
+      </c>
       <c r="AM5" s="2"/>
       <c r="AN5" s="2"/>
       <c r="AO5" s="2"/>
       <c r="AP5" s="2"/>
       <c r="AQ5" s="2"/>
-      <c r="AR5" s="4"/>
+      <c r="AR5" s="2"/>
       <c r="AS5" s="4"/>
+      <c r="AT5" s="4"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -2489,38 +2517,38 @@
         <v>434</v>
       </c>
       <c r="X6" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y6" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="Z6" s="2">
         <v>123</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="AA6" s="2">
         <v>2908</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="AB6" s="2">
         <v>2003</v>
       </c>
-      <c r="AB6" s="4" t="s">
+      <c r="AC6" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="AC6" s="4" t="s">
+      <c r="AD6" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="AD6" s="2" t="s">
+      <c r="AE6" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="AE6" s="2">
-        <v>1</v>
-      </c>
       <c r="AF6" s="2">
         <v>1</v>
       </c>
-      <c r="AG6" s="2"/>
-      <c r="AH6" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="2"/>
       <c r="AI6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ6" s="2">
         <v>1</v>
@@ -2528,16 +2556,19 @@
       <c r="AK6" s="2">
         <v>1</v>
       </c>
-      <c r="AL6" s="2"/>
+      <c r="AL6" s="2">
+        <v>1</v>
+      </c>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
       <c r="AO6" s="2"/>
       <c r="AP6" s="2"/>
       <c r="AQ6" s="2"/>
-      <c r="AR6" s="4"/>
+      <c r="AR6" s="2"/>
       <c r="AS6" s="4"/>
+      <c r="AT6" s="4"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -2606,38 +2637,38 @@
         <v>435</v>
       </c>
       <c r="X7" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y7" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="Y7" s="2">
+      <c r="Z7" s="2">
         <v>123</v>
       </c>
-      <c r="Z7" s="2">
+      <c r="AA7" s="2">
         <v>2908</v>
       </c>
-      <c r="AA7" s="2">
+      <c r="AB7" s="2">
         <v>2003</v>
       </c>
-      <c r="AB7" s="4" t="s">
+      <c r="AC7" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="AC7" s="4" t="s">
+      <c r="AD7" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="AD7" s="2" t="s">
+      <c r="AE7" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="AE7" s="2">
-        <v>1</v>
-      </c>
       <c r="AF7" s="2">
         <v>1</v>
       </c>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH7" s="2"/>
       <c r="AI7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ7" s="2">
         <v>1</v>
@@ -2645,16 +2676,19 @@
       <c r="AK7" s="2">
         <v>1</v>
       </c>
-      <c r="AL7" s="2"/>
+      <c r="AL7" s="2">
+        <v>1</v>
+      </c>
       <c r="AM7" s="2"/>
       <c r="AN7" s="2"/>
       <c r="AO7" s="2"/>
       <c r="AP7" s="2"/>
       <c r="AQ7" s="2"/>
-      <c r="AR7" s="4"/>
+      <c r="AR7" s="2"/>
       <c r="AS7" s="4"/>
+      <c r="AT7" s="4"/>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -2723,38 +2757,38 @@
         <v>436</v>
       </c>
       <c r="X8" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y8" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="Z8" s="2">
         <v>123</v>
       </c>
-      <c r="Z8" s="2">
+      <c r="AA8" s="2">
         <v>2908</v>
       </c>
-      <c r="AA8" s="2">
+      <c r="AB8" s="2">
         <v>2003</v>
       </c>
-      <c r="AB8" s="4" t="s">
+      <c r="AC8" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="AC8" s="4" t="s">
+      <c r="AD8" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="AD8" s="2" t="s">
+      <c r="AE8" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="AE8" s="2">
-        <v>1</v>
-      </c>
       <c r="AF8" s="2">
         <v>1</v>
       </c>
-      <c r="AG8" s="2"/>
-      <c r="AH8" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="2"/>
       <c r="AI8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ8" s="2">
         <v>1</v>
@@ -2762,16 +2796,19 @@
       <c r="AK8" s="2">
         <v>1</v>
       </c>
-      <c r="AL8" s="2"/>
+      <c r="AL8" s="2">
+        <v>1</v>
+      </c>
       <c r="AM8" s="2"/>
       <c r="AN8" s="2"/>
       <c r="AO8" s="2"/>
       <c r="AP8" s="2"/>
       <c r="AQ8" s="2"/>
-      <c r="AR8" s="4"/>
+      <c r="AR8" s="2"/>
       <c r="AS8" s="4"/>
+      <c r="AT8" s="4"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>3</v>
       </c>
@@ -2840,38 +2877,38 @@
         <v>437</v>
       </c>
       <c r="X9" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y9" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="Z9" s="2">
         <v>123</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="AA9" s="2">
         <v>2908</v>
       </c>
-      <c r="AA9" s="2">
+      <c r="AB9" s="2">
         <v>2003</v>
       </c>
-      <c r="AB9" s="4" t="s">
+      <c r="AC9" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="AC9" s="4" t="s">
+      <c r="AD9" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="AD9" s="2" t="s">
+      <c r="AE9" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="AE9" s="2">
-        <v>1</v>
-      </c>
       <c r="AF9" s="2">
         <v>1</v>
       </c>
-      <c r="AG9" s="2"/>
-      <c r="AH9" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="2"/>
       <c r="AI9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ9" s="2">
         <v>1</v>
@@ -2879,16 +2916,19 @@
       <c r="AK9" s="2">
         <v>1</v>
       </c>
-      <c r="AL9" s="2"/>
+      <c r="AL9" s="2">
+        <v>1</v>
+      </c>
       <c r="AM9" s="2"/>
       <c r="AN9" s="2"/>
       <c r="AO9" s="2"/>
       <c r="AP9" s="2"/>
       <c r="AQ9" s="2"/>
-      <c r="AR9" s="4"/>
+      <c r="AR9" s="2"/>
       <c r="AS9" s="4"/>
+      <c r="AT9" s="4"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>3</v>
       </c>
@@ -2957,38 +2997,38 @@
         <v>438</v>
       </c>
       <c r="X10" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y10" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="Y10" s="2">
+      <c r="Z10" s="2">
         <v>123</v>
       </c>
-      <c r="Z10" s="2">
+      <c r="AA10" s="2">
         <v>2908</v>
       </c>
-      <c r="AA10" s="2">
+      <c r="AB10" s="2">
         <v>2003</v>
       </c>
-      <c r="AB10" s="4" t="s">
+      <c r="AC10" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="AC10" s="4" t="s">
+      <c r="AD10" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="AD10" s="2" t="s">
+      <c r="AE10" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="AE10" s="2">
-        <v>1</v>
-      </c>
       <c r="AF10" s="2">
         <v>1</v>
       </c>
-      <c r="AG10" s="2"/>
-      <c r="AH10" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="2"/>
       <c r="AI10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ10" s="2">
         <v>1</v>
@@ -2996,16 +3036,19 @@
       <c r="AK10" s="2">
         <v>1</v>
       </c>
-      <c r="AL10" s="2"/>
+      <c r="AL10" s="2">
+        <v>1</v>
+      </c>
       <c r="AM10" s="2"/>
       <c r="AN10" s="2"/>
       <c r="AO10" s="2"/>
       <c r="AP10" s="2"/>
       <c r="AQ10" s="2"/>
-      <c r="AR10" s="4"/>
+      <c r="AR10" s="2"/>
       <c r="AS10" s="4"/>
+      <c r="AT10" s="4"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -3074,38 +3117,38 @@
         <v>439</v>
       </c>
       <c r="X11" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y11" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="Y11" s="2">
+      <c r="Z11" s="2">
         <v>123</v>
       </c>
-      <c r="Z11" s="2">
+      <c r="AA11" s="2">
         <v>2908</v>
       </c>
-      <c r="AA11" s="2">
+      <c r="AB11" s="2">
         <v>2003</v>
       </c>
-      <c r="AB11" s="4" t="s">
+      <c r="AC11" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="AC11" s="4" t="s">
+      <c r="AD11" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="AD11" s="2" t="s">
+      <c r="AE11" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="AE11" s="2">
-        <v>1</v>
-      </c>
       <c r="AF11" s="2">
         <v>1</v>
       </c>
-      <c r="AG11" s="2"/>
-      <c r="AH11" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG11" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH11" s="2"/>
       <c r="AI11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ11" s="2">
         <v>1</v>
@@ -3113,16 +3156,19 @@
       <c r="AK11" s="2">
         <v>1</v>
       </c>
-      <c r="AL11" s="2"/>
+      <c r="AL11" s="2">
+        <v>1</v>
+      </c>
       <c r="AM11" s="2"/>
       <c r="AN11" s="2"/>
       <c r="AO11" s="2"/>
       <c r="AP11" s="2"/>
       <c r="AQ11" s="2"/>
-      <c r="AR11" s="4"/>
+      <c r="AR11" s="2"/>
       <c r="AS11" s="4"/>
+      <c r="AT11" s="4"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -3191,38 +3237,38 @@
         <v>440</v>
       </c>
       <c r="X12" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y12" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="Y12" s="2">
+      <c r="Z12" s="2">
         <v>123</v>
       </c>
-      <c r="Z12" s="2">
+      <c r="AA12" s="2">
         <v>2908</v>
       </c>
-      <c r="AA12" s="2">
+      <c r="AB12" s="2">
         <v>2003</v>
       </c>
-      <c r="AB12" s="4" t="s">
+      <c r="AC12" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="AC12" s="4" t="s">
+      <c r="AD12" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="AD12" s="2" t="s">
+      <c r="AE12" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="AE12" s="2">
-        <v>1</v>
-      </c>
       <c r="AF12" s="2">
         <v>1</v>
       </c>
-      <c r="AG12" s="2"/>
-      <c r="AH12" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG12" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH12" s="2"/>
       <c r="AI12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ12" s="2">
         <v>1</v>
@@ -3230,16 +3276,19 @@
       <c r="AK12" s="2">
         <v>1</v>
       </c>
-      <c r="AL12" s="2"/>
+      <c r="AL12" s="2">
+        <v>1</v>
+      </c>
       <c r="AM12" s="2"/>
       <c r="AN12" s="2"/>
       <c r="AO12" s="2"/>
       <c r="AP12" s="2"/>
       <c r="AQ12" s="2"/>
-      <c r="AR12" s="4"/>
+      <c r="AR12" s="2"/>
       <c r="AS12" s="4"/>
+      <c r="AT12" s="4"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -3293,7 +3342,7 @@
         <v>5</v>
       </c>
       <c r="S13" s="2">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="T13" s="2" t="s">
         <v>464</v>
@@ -3308,38 +3357,38 @@
         <v>441</v>
       </c>
       <c r="X13" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="Y13" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="Y13" s="2">
+      <c r="Z13" s="2">
         <v>123</v>
       </c>
-      <c r="Z13" s="2">
+      <c r="AA13" s="2">
         <v>2908</v>
       </c>
-      <c r="AA13" s="2">
+      <c r="AB13" s="2">
         <v>2003</v>
       </c>
-      <c r="AB13" s="4" t="s">
+      <c r="AC13" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="AC13" s="4" t="s">
+      <c r="AD13" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="AD13" s="2" t="s">
+      <c r="AE13" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="AE13" s="2">
-        <v>1</v>
-      </c>
       <c r="AF13" s="2">
         <v>1</v>
       </c>
-      <c r="AG13" s="2"/>
-      <c r="AH13" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH13" s="2"/>
       <c r="AI13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ13" s="2">
         <v>1</v>
@@ -3347,16 +3396,19 @@
       <c r="AK13" s="2">
         <v>1</v>
       </c>
-      <c r="AL13" s="2"/>
+      <c r="AL13" s="2">
+        <v>1</v>
+      </c>
       <c r="AM13" s="2"/>
       <c r="AN13" s="2"/>
       <c r="AO13" s="2"/>
       <c r="AP13" s="2"/>
       <c r="AQ13" s="2"/>
-      <c r="AR13" s="4"/>
+      <c r="AR13" s="2"/>
       <c r="AS13" s="4"/>
+      <c r="AT13" s="4"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>3</v>
       </c>
@@ -3410,7 +3462,7 @@
         <v>8</v>
       </c>
       <c r="S14" s="2">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="T14" s="2" t="s">
         <v>464</v>
@@ -3425,38 +3477,38 @@
         <v>442</v>
       </c>
       <c r="X14" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="Y14" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="Y14" s="2">
+      <c r="Z14" s="2">
         <v>123</v>
       </c>
-      <c r="Z14" s="2">
+      <c r="AA14" s="2">
         <v>2908</v>
       </c>
-      <c r="AA14" s="2">
+      <c r="AB14" s="2">
         <v>2003</v>
       </c>
-      <c r="AB14" s="4" t="s">
+      <c r="AC14" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="AC14" s="4" t="s">
+      <c r="AD14" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="AD14" s="2" t="s">
+      <c r="AE14" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="AE14" s="2">
-        <v>1</v>
-      </c>
       <c r="AF14" s="2">
         <v>1</v>
       </c>
-      <c r="AG14" s="2"/>
-      <c r="AH14" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG14" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH14" s="2"/>
       <c r="AI14" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ14" s="2">
         <v>1</v>
@@ -3464,16 +3516,19 @@
       <c r="AK14" s="2">
         <v>1</v>
       </c>
-      <c r="AL14" s="2"/>
+      <c r="AL14" s="2">
+        <v>1</v>
+      </c>
       <c r="AM14" s="2"/>
       <c r="AN14" s="2"/>
       <c r="AO14" s="2"/>
       <c r="AP14" s="2"/>
       <c r="AQ14" s="2"/>
-      <c r="AR14" s="4"/>
+      <c r="AR14" s="2"/>
       <c r="AS14" s="4"/>
+      <c r="AT14" s="4"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -3527,7 +3582,7 @@
         <v>1</v>
       </c>
       <c r="S15" s="2">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="T15" s="2" t="s">
         <v>464</v>
@@ -3542,38 +3597,38 @@
         <v>443</v>
       </c>
       <c r="X15" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="Y15" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="Y15" s="2">
+      <c r="Z15" s="2">
         <v>123</v>
       </c>
-      <c r="Z15" s="2">
+      <c r="AA15" s="2">
         <v>2908</v>
       </c>
-      <c r="AA15" s="2">
+      <c r="AB15" s="2">
         <v>2003</v>
       </c>
-      <c r="AB15" s="4" t="s">
+      <c r="AC15" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="AC15" s="4" t="s">
+      <c r="AD15" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="AD15" s="2" t="s">
+      <c r="AE15" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="AE15" s="2">
-        <v>1</v>
-      </c>
       <c r="AF15" s="2">
         <v>1</v>
       </c>
-      <c r="AG15" s="2"/>
-      <c r="AH15" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG15" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH15" s="2"/>
       <c r="AI15" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ15" s="2">
         <v>1</v>
@@ -3581,16 +3636,19 @@
       <c r="AK15" s="2">
         <v>1</v>
       </c>
-      <c r="AL15" s="2"/>
+      <c r="AL15" s="2">
+        <v>1</v>
+      </c>
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
       <c r="AO15" s="2"/>
       <c r="AP15" s="2"/>
       <c r="AQ15" s="2"/>
-      <c r="AR15" s="4"/>
+      <c r="AR15" s="2"/>
       <c r="AS15" s="4"/>
+      <c r="AT15" s="4"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>3</v>
       </c>
@@ -3644,7 +3702,7 @@
         <v>2</v>
       </c>
       <c r="S16" s="2">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="T16" s="2" t="s">
         <v>464</v>
@@ -3659,38 +3717,38 @@
         <v>444</v>
       </c>
       <c r="X16" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="Y16" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="Y16" s="2">
+      <c r="Z16" s="2">
         <v>123</v>
       </c>
-      <c r="Z16" s="2">
+      <c r="AA16" s="2">
         <v>2908</v>
       </c>
-      <c r="AA16" s="2">
+      <c r="AB16" s="2">
         <v>2003</v>
       </c>
-      <c r="AB16" s="4" t="s">
+      <c r="AC16" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="AC16" s="4" t="s">
+      <c r="AD16" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="AD16" s="2" t="s">
+      <c r="AE16" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="AE16" s="2">
-        <v>1</v>
-      </c>
       <c r="AF16" s="2">
         <v>1</v>
       </c>
-      <c r="AG16" s="2"/>
-      <c r="AH16" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH16" s="2"/>
       <c r="AI16" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ16" s="2">
         <v>1</v>
@@ -3698,28 +3756,31 @@
       <c r="AK16" s="2">
         <v>1</v>
       </c>
-      <c r="AL16" s="6" t="s">
+      <c r="AL16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AM16" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="AM16" s="6" t="s">
+      <c r="AN16" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="AN16" s="2" t="s">
+      <c r="AO16" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="AO16" s="2" t="s">
+      <c r="AP16" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="AP16" s="2">
+      <c r="AQ16" s="2">
         <v>98</v>
       </c>
-      <c r="AQ16" s="2">
-        <v>2</v>
-      </c>
-      <c r="AR16" s="4"/>
+      <c r="AR16" s="2">
+        <v>2</v>
+      </c>
       <c r="AS16" s="4"/>
+      <c r="AT16" s="4"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>3</v>
       </c>
@@ -3788,38 +3849,38 @@
         <v>445</v>
       </c>
       <c r="X17" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y17" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="Y17" s="2">
+      <c r="Z17" s="2">
         <v>123</v>
       </c>
-      <c r="Z17" s="2">
+      <c r="AA17" s="2">
         <v>2908</v>
       </c>
-      <c r="AA17" s="2">
+      <c r="AB17" s="2">
         <v>2003</v>
       </c>
-      <c r="AB17" s="4" t="s">
+      <c r="AC17" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="AC17" s="4" t="s">
+      <c r="AD17" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="AD17" s="2" t="s">
+      <c r="AE17" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="AE17" s="2">
-        <v>1</v>
-      </c>
       <c r="AF17" s="2">
         <v>1</v>
       </c>
-      <c r="AG17" s="2"/>
-      <c r="AH17" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG17" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH17" s="2"/>
       <c r="AI17" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ17" s="2">
         <v>1</v>
@@ -3827,28 +3888,31 @@
       <c r="AK17" s="2">
         <v>1</v>
       </c>
-      <c r="AL17" s="6" t="s">
+      <c r="AL17" s="2">
+        <v>1</v>
+      </c>
+      <c r="AM17" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="AM17" s="6" t="s">
+      <c r="AN17" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="AN17" s="2" t="s">
+      <c r="AO17" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="AO17" s="2" t="s">
+      <c r="AP17" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="AP17" s="2">
+      <c r="AQ17" s="2">
         <v>98</v>
       </c>
-      <c r="AQ17" s="2">
-        <v>2</v>
-      </c>
-      <c r="AR17" s="4"/>
+      <c r="AR17" s="2">
+        <v>2</v>
+      </c>
       <c r="AS17" s="4"/>
+      <c r="AT17" s="4"/>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>3</v>
       </c>
@@ -3917,38 +3981,38 @@
         <v>446</v>
       </c>
       <c r="X18" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y18" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="Y18" s="2">
+      <c r="Z18" s="2">
         <v>123</v>
       </c>
-      <c r="Z18" s="2">
+      <c r="AA18" s="2">
         <v>2908</v>
       </c>
-      <c r="AA18" s="2">
+      <c r="AB18" s="2">
         <v>2003</v>
       </c>
-      <c r="AB18" s="4" t="s">
+      <c r="AC18" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="AC18" s="4" t="s">
+      <c r="AD18" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="AD18" s="2" t="s">
+      <c r="AE18" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="AE18" s="2">
-        <v>1</v>
-      </c>
       <c r="AF18" s="2">
         <v>1</v>
       </c>
-      <c r="AG18" s="2"/>
-      <c r="AH18" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG18" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH18" s="2"/>
       <c r="AI18" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ18" s="2">
         <v>1</v>
@@ -3956,28 +4020,31 @@
       <c r="AK18" s="2">
         <v>1</v>
       </c>
-      <c r="AL18" s="6" t="s">
+      <c r="AL18" s="2">
+        <v>1</v>
+      </c>
+      <c r="AM18" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="AM18" s="6" t="s">
+      <c r="AN18" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="AN18" s="2" t="s">
+      <c r="AO18" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="AO18" s="2" t="s">
+      <c r="AP18" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="AP18" s="2">
+      <c r="AQ18" s="2">
         <v>98</v>
       </c>
-      <c r="AQ18" s="2">
-        <v>2</v>
-      </c>
-      <c r="AR18" s="4"/>
+      <c r="AR18" s="2">
+        <v>2</v>
+      </c>
       <c r="AS18" s="4"/>
+      <c r="AT18" s="4"/>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>3</v>
       </c>
@@ -4046,38 +4113,38 @@
         <v>447</v>
       </c>
       <c r="X19" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y19" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="Y19" s="2">
+      <c r="Z19" s="2">
         <v>123</v>
       </c>
-      <c r="Z19" s="2">
+      <c r="AA19" s="2">
         <v>2908</v>
       </c>
-      <c r="AA19" s="2">
+      <c r="AB19" s="2">
         <v>2003</v>
       </c>
-      <c r="AB19" s="4" t="s">
+      <c r="AC19" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="AC19" s="4" t="s">
+      <c r="AD19" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="AD19" s="2" t="s">
+      <c r="AE19" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="AE19" s="2">
-        <v>1</v>
-      </c>
       <c r="AF19" s="2">
         <v>1</v>
       </c>
-      <c r="AG19" s="2"/>
-      <c r="AH19" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG19" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH19" s="2"/>
       <c r="AI19" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ19" s="2">
         <v>1</v>
@@ -4085,28 +4152,31 @@
       <c r="AK19" s="2">
         <v>1</v>
       </c>
-      <c r="AL19" s="6" t="s">
+      <c r="AL19" s="2">
+        <v>1</v>
+      </c>
+      <c r="AM19" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="AM19" s="6" t="s">
+      <c r="AN19" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="AN19" s="2" t="s">
+      <c r="AO19" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="AO19" s="2" t="s">
+      <c r="AP19" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="AP19" s="2">
+      <c r="AQ19" s="2">
         <v>98</v>
       </c>
-      <c r="AQ19" s="2">
-        <v>2</v>
-      </c>
-      <c r="AR19" s="4"/>
+      <c r="AR19" s="2">
+        <v>2</v>
+      </c>
       <c r="AS19" s="4"/>
+      <c r="AT19" s="4"/>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>3</v>
       </c>
@@ -4160,7 +4230,7 @@
         <v>12</v>
       </c>
       <c r="S20" s="2">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="T20" s="2" t="s">
         <v>464</v>
@@ -4175,38 +4245,38 @@
         <v>448</v>
       </c>
       <c r="X20" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="Y20" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="Y20" s="2">
+      <c r="Z20" s="2">
         <v>123</v>
       </c>
-      <c r="Z20" s="2">
+      <c r="AA20" s="2">
         <v>2908</v>
       </c>
-      <c r="AA20" s="2">
+      <c r="AB20" s="2">
         <v>2003</v>
       </c>
-      <c r="AB20" s="4" t="s">
+      <c r="AC20" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="AC20" s="4" t="s">
+      <c r="AD20" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="AD20" s="2" t="s">
+      <c r="AE20" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="AE20" s="2">
-        <v>1</v>
-      </c>
       <c r="AF20" s="2">
         <v>1</v>
       </c>
-      <c r="AG20" s="2"/>
-      <c r="AH20" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG20" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH20" s="2"/>
       <c r="AI20" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ20" s="2">
         <v>1</v>
@@ -4214,28 +4284,31 @@
       <c r="AK20" s="2">
         <v>1</v>
       </c>
-      <c r="AL20" s="6" t="s">
+      <c r="AL20" s="2">
+        <v>1</v>
+      </c>
+      <c r="AM20" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="AM20" s="6" t="s">
+      <c r="AN20" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="AN20" s="2" t="s">
+      <c r="AO20" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="AO20" s="2" t="s">
+      <c r="AP20" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="AP20" s="2">
+      <c r="AQ20" s="2">
         <v>98</v>
       </c>
-      <c r="AQ20" s="2">
-        <v>2</v>
-      </c>
-      <c r="AR20" s="4"/>
+      <c r="AR20" s="2">
+        <v>2</v>
+      </c>
       <c r="AS20" s="4"/>
+      <c r="AT20" s="4"/>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>3</v>
       </c>
@@ -4289,7 +4362,7 @@
         <v>14</v>
       </c>
       <c r="S21" s="2">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="T21" s="2" t="s">
         <v>464</v>
@@ -4304,38 +4377,38 @@
         <v>449</v>
       </c>
       <c r="X21" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="Y21" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="Y21" s="2">
+      <c r="Z21" s="2">
         <v>123</v>
       </c>
-      <c r="Z21" s="2">
+      <c r="AA21" s="2">
         <v>2908</v>
       </c>
-      <c r="AA21" s="2">
+      <c r="AB21" s="2">
         <v>2003</v>
       </c>
-      <c r="AB21" s="4" t="s">
+      <c r="AC21" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="AC21" s="4" t="s">
+      <c r="AD21" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="AD21" s="2" t="s">
+      <c r="AE21" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="AE21" s="2">
-        <v>1</v>
-      </c>
       <c r="AF21" s="2">
         <v>1</v>
       </c>
-      <c r="AG21" s="2"/>
-      <c r="AH21" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG21" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH21" s="2"/>
       <c r="AI21" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ21" s="2">
         <v>1</v>
@@ -4343,28 +4416,31 @@
       <c r="AK21" s="2">
         <v>1</v>
       </c>
-      <c r="AL21" s="6" t="s">
+      <c r="AL21" s="2">
+        <v>1</v>
+      </c>
+      <c r="AM21" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="AM21" s="6" t="s">
+      <c r="AN21" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="AN21" s="2" t="s">
+      <c r="AO21" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="AO21" s="2" t="s">
+      <c r="AP21" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="AP21" s="2">
+      <c r="AQ21" s="2">
         <v>98</v>
       </c>
-      <c r="AQ21" s="2">
-        <v>2</v>
-      </c>
-      <c r="AR21" s="4"/>
+      <c r="AR21" s="2">
+        <v>2</v>
+      </c>
       <c r="AS21" s="4"/>
+      <c r="AT21" s="4"/>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>3</v>
       </c>
@@ -4418,7 +4494,7 @@
         <v>1</v>
       </c>
       <c r="S22" s="2">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="T22" s="2" t="s">
         <v>464</v>
@@ -4433,38 +4509,38 @@
         <v>450</v>
       </c>
       <c r="X22" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="Y22" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="Y22" s="2">
+      <c r="Z22" s="2">
         <v>123</v>
       </c>
-      <c r="Z22" s="2">
+      <c r="AA22" s="2">
         <v>2908</v>
       </c>
-      <c r="AA22" s="2">
+      <c r="AB22" s="2">
         <v>2003</v>
       </c>
-      <c r="AB22" s="4" t="s">
+      <c r="AC22" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="AC22" s="4" t="s">
+      <c r="AD22" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="AD22" s="2" t="s">
+      <c r="AE22" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="AE22" s="2">
-        <v>1</v>
-      </c>
       <c r="AF22" s="2">
         <v>1</v>
       </c>
-      <c r="AG22" s="2"/>
-      <c r="AH22" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG22" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH22" s="2"/>
       <c r="AI22" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ22" s="2">
         <v>1</v>
@@ -4472,16 +4548,19 @@
       <c r="AK22" s="2">
         <v>1</v>
       </c>
-      <c r="AL22" s="2"/>
+      <c r="AL22" s="2">
+        <v>1</v>
+      </c>
       <c r="AM22" s="2"/>
       <c r="AN22" s="2"/>
       <c r="AO22" s="2"/>
       <c r="AP22" s="2"/>
       <c r="AQ22" s="2"/>
-      <c r="AR22" s="4"/>
+      <c r="AR22" s="2"/>
       <c r="AS22" s="4"/>
+      <c r="AT22" s="4"/>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>3</v>
       </c>
@@ -4535,7 +4614,7 @@
         <v>1</v>
       </c>
       <c r="S23" s="2">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="T23" s="2" t="s">
         <v>464</v>
@@ -4550,38 +4629,38 @@
         <v>451</v>
       </c>
       <c r="X23" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="Y23" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="Y23" s="2">
+      <c r="Z23" s="2">
         <v>123</v>
       </c>
-      <c r="Z23" s="2">
+      <c r="AA23" s="2">
         <v>2908</v>
       </c>
-      <c r="AA23" s="2">
+      <c r="AB23" s="2">
         <v>2003</v>
       </c>
-      <c r="AB23" s="4" t="s">
+      <c r="AC23" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="AC23" s="4" t="s">
+      <c r="AD23" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="AD23" s="2" t="s">
+      <c r="AE23" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="AE23" s="2">
-        <v>1</v>
-      </c>
       <c r="AF23" s="2">
         <v>1</v>
       </c>
-      <c r="AG23" s="2"/>
-      <c r="AH23" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG23" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH23" s="2"/>
       <c r="AI23" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ23" s="2">
         <v>1</v>
@@ -4589,16 +4668,19 @@
       <c r="AK23" s="2">
         <v>1</v>
       </c>
-      <c r="AL23" s="2"/>
+      <c r="AL23" s="2">
+        <v>1</v>
+      </c>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
       <c r="AO23" s="2"/>
       <c r="AP23" s="2"/>
       <c r="AQ23" s="2"/>
-      <c r="AR23" s="4"/>
+      <c r="AR23" s="2"/>
       <c r="AS23" s="4"/>
+      <c r="AT23" s="4"/>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>3</v>
       </c>
@@ -4652,7 +4734,7 @@
         <v>1</v>
       </c>
       <c r="S24" s="2">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="T24" s="2" t="s">
         <v>464</v>
@@ -4667,38 +4749,38 @@
         <v>452</v>
       </c>
       <c r="X24" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="Y24" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="Y24" s="2">
+      <c r="Z24" s="2">
         <v>123</v>
       </c>
-      <c r="Z24" s="2">
+      <c r="AA24" s="2">
         <v>2908</v>
       </c>
-      <c r="AA24" s="2">
+      <c r="AB24" s="2">
         <v>2003</v>
       </c>
-      <c r="AB24" s="4" t="s">
+      <c r="AC24" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="AC24" s="4" t="s">
+      <c r="AD24" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="AD24" s="2" t="s">
+      <c r="AE24" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="AE24" s="2">
-        <v>1</v>
-      </c>
       <c r="AF24" s="2">
         <v>1</v>
       </c>
-      <c r="AG24" s="2"/>
-      <c r="AH24" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG24" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH24" s="2"/>
       <c r="AI24" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ24" s="2">
         <v>1</v>
@@ -4706,16 +4788,19 @@
       <c r="AK24" s="2">
         <v>1</v>
       </c>
-      <c r="AL24" s="2"/>
+      <c r="AL24" s="2">
+        <v>1</v>
+      </c>
       <c r="AM24" s="2"/>
       <c r="AN24" s="2"/>
       <c r="AO24" s="2"/>
       <c r="AP24" s="2"/>
       <c r="AQ24" s="2"/>
-      <c r="AR24" s="4"/>
+      <c r="AR24" s="2"/>
       <c r="AS24" s="4"/>
+      <c r="AT24" s="4"/>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>3</v>
       </c>
@@ -4780,38 +4865,38 @@
         <v>453</v>
       </c>
       <c r="X25" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y25" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="Y25" s="2">
+      <c r="Z25" s="2">
         <v>123</v>
       </c>
-      <c r="Z25" s="2">
+      <c r="AA25" s="2">
         <v>2908</v>
       </c>
-      <c r="AA25" s="2">
+      <c r="AB25" s="2">
         <v>2003</v>
       </c>
-      <c r="AB25" s="4" t="s">
+      <c r="AC25" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="AC25" s="4" t="s">
+      <c r="AD25" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="AD25" s="2" t="s">
+      <c r="AE25" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="AE25" s="2">
-        <v>1</v>
-      </c>
       <c r="AF25" s="2">
         <v>1</v>
       </c>
-      <c r="AG25" s="2"/>
-      <c r="AH25" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG25" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH25" s="2"/>
       <c r="AI25" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ25" s="2">
         <v>1</v>
@@ -4819,16 +4904,19 @@
       <c r="AK25" s="2">
         <v>1</v>
       </c>
-      <c r="AL25" s="2"/>
+      <c r="AL25" s="2">
+        <v>1</v>
+      </c>
       <c r="AM25" s="2"/>
       <c r="AN25" s="2"/>
       <c r="AO25" s="2"/>
       <c r="AP25" s="2"/>
       <c r="AQ25" s="2"/>
-      <c r="AR25" s="4"/>
+      <c r="AR25" s="2"/>
       <c r="AS25" s="4"/>
+      <c r="AT25" s="4"/>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>3</v>
       </c>
@@ -4893,38 +4981,38 @@
         <v>454</v>
       </c>
       <c r="X26" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y26" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="Y26" s="2">
+      <c r="Z26" s="2">
         <v>123</v>
       </c>
-      <c r="Z26" s="2">
+      <c r="AA26" s="2">
         <v>2908</v>
       </c>
-      <c r="AA26" s="2">
+      <c r="AB26" s="2">
         <v>2003</v>
       </c>
-      <c r="AB26" s="4" t="s">
+      <c r="AC26" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="AC26" s="4" t="s">
+      <c r="AD26" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="AD26" s="2" t="s">
+      <c r="AE26" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="AE26" s="2">
-        <v>1</v>
-      </c>
       <c r="AF26" s="2">
         <v>1</v>
       </c>
-      <c r="AG26" s="2"/>
-      <c r="AH26" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG26" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH26" s="2"/>
       <c r="AI26" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ26" s="2">
         <v>1</v>
@@ -4932,16 +5020,19 @@
       <c r="AK26" s="2">
         <v>1</v>
       </c>
-      <c r="AL26" s="2"/>
+      <c r="AL26" s="2">
+        <v>1</v>
+      </c>
       <c r="AM26" s="2"/>
       <c r="AN26" s="2"/>
       <c r="AO26" s="2"/>
       <c r="AP26" s="2"/>
       <c r="AQ26" s="2"/>
-      <c r="AR26" s="4"/>
+      <c r="AR26" s="2"/>
       <c r="AS26" s="4"/>
+      <c r="AT26" s="4"/>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>3</v>
       </c>
@@ -5006,38 +5097,38 @@
         <v>455</v>
       </c>
       <c r="X27" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y27" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="Y27" s="2">
+      <c r="Z27" s="2">
         <v>123</v>
       </c>
-      <c r="Z27" s="2">
+      <c r="AA27" s="2">
         <v>2908</v>
       </c>
-      <c r="AA27" s="2">
+      <c r="AB27" s="2">
         <v>2003</v>
       </c>
-      <c r="AB27" s="4" t="s">
+      <c r="AC27" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="AC27" s="4" t="s">
+      <c r="AD27" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="AD27" s="2" t="s">
+      <c r="AE27" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="AE27" s="2">
-        <v>1</v>
-      </c>
       <c r="AF27" s="2">
         <v>1</v>
       </c>
-      <c r="AG27" s="2"/>
-      <c r="AH27" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG27" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH27" s="2"/>
       <c r="AI27" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ27" s="2">
         <v>1</v>
@@ -5045,16 +5136,19 @@
       <c r="AK27" s="2">
         <v>1</v>
       </c>
-      <c r="AL27" s="2"/>
+      <c r="AL27" s="2">
+        <v>1</v>
+      </c>
       <c r="AM27" s="2"/>
       <c r="AN27" s="2"/>
       <c r="AO27" s="2"/>
       <c r="AP27" s="2"/>
       <c r="AQ27" s="2"/>
-      <c r="AR27" s="4"/>
+      <c r="AR27" s="2"/>
       <c r="AS27" s="4"/>
+      <c r="AT27" s="4"/>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>3</v>
       </c>
@@ -5119,38 +5213,38 @@
         <v>456</v>
       </c>
       <c r="X28" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y28" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="Y28" s="2">
+      <c r="Z28" s="2">
         <v>123</v>
       </c>
-      <c r="Z28" s="2">
+      <c r="AA28" s="2">
         <v>2908</v>
       </c>
-      <c r="AA28" s="2">
+      <c r="AB28" s="2">
         <v>2003</v>
       </c>
-      <c r="AB28" s="4" t="s">
+      <c r="AC28" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="AC28" s="4" t="s">
+      <c r="AD28" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="AD28" s="2" t="s">
+      <c r="AE28" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="AE28" s="2">
-        <v>1</v>
-      </c>
       <c r="AF28" s="2">
         <v>1</v>
       </c>
-      <c r="AG28" s="2"/>
-      <c r="AH28" s="2">
-        <v>2</v>
-      </c>
+      <c r="AG28" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH28" s="2"/>
       <c r="AI28" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ28" s="2">
         <v>1</v>
@@ -5158,17 +5252,20 @@
       <c r="AK28" s="2">
         <v>1</v>
       </c>
-      <c r="AL28" s="2"/>
+      <c r="AL28" s="2">
+        <v>1</v>
+      </c>
       <c r="AM28" s="2"/>
       <c r="AN28" s="2"/>
       <c r="AO28" s="2"/>
       <c r="AP28" s="2"/>
       <c r="AQ28" s="2"/>
-      <c r="AR28" s="4"/>
+      <c r="AR28" s="2"/>
       <c r="AS28" s="4"/>
+      <c r="AT28" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:AH28"/>
+  <autoFilter ref="B1:AI28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>